<commit_message>
Problems 1-4 done, 5-7  next
</commit_message>
<xml_diff>
--- a/The_Maps_Case.xlsx
+++ b/The_Maps_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D647C2-E5A4-4C66-A179-E17E823C9DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74973EAC-1F9C-4944-81D5-AB91336990B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="210">
   <si>
     <t>Case Author</t>
   </si>
@@ -1551,6 +1551,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>195100</xdr:colOff>
+      <xdr:row>154</xdr:row>
+      <xdr:rowOff>137224</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9FB46C0-93DD-B618-F92D-15B7A569B1E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12412980" y="38762940"/>
+          <a:ext cx="5658640" cy="457264"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1971,8 +2015,8 @@
   </sheetPr>
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E148" sqref="E148"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G223" sqref="G223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -3894,7 +3938,7 @@
       <c r="H144" s="7"/>
       <c r="I144" s="16"/>
     </row>
-    <row r="145" spans="2:8" ht="15" customHeight="1">
+    <row r="145" spans="2:11" ht="15" customHeight="1">
       <c r="B145" s="18" t="s">
         <v>123</v>
       </c>
@@ -3904,35 +3948,35 @@
       <c r="G145" s="7"/>
       <c r="H145" s="7"/>
     </row>
-    <row r="146" spans="2:8" ht="15" customHeight="1">
+    <row r="146" spans="2:11" ht="15" customHeight="1">
       <c r="B146" s="18"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="29"/>
       <c r="G146" s="21"/>
     </row>
-    <row r="147" spans="2:8" ht="15" customHeight="1">
+    <row r="147" spans="2:11" ht="15" customHeight="1">
       <c r="B147" s="18"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="29"/>
       <c r="G147" s="21"/>
     </row>
-    <row r="148" spans="2:8" ht="15" customHeight="1">
+    <row r="148" spans="2:11" ht="15" customHeight="1">
       <c r="B148" s="18"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="29"/>
       <c r="G148" s="21"/>
     </row>
-    <row r="149" spans="2:8" ht="15" customHeight="1">
+    <row r="149" spans="2:11" ht="15" customHeight="1">
       <c r="B149" s="18"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="29"/>
       <c r="G149" s="21"/>
     </row>
-    <row r="150" spans="2:8" ht="15" customHeight="1">
+    <row r="150" spans="2:11" ht="15" customHeight="1">
       <c r="B150" s="18" t="s">
         <v>124</v>
       </c>
@@ -3940,8 +3984,11 @@
       <c r="D150" s="7"/>
       <c r="E150" s="29"/>
       <c r="G150" s="21"/>
-    </row>
-    <row r="151" spans="2:8" ht="15" customHeight="1">
+      <c r="I150" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="151" spans="2:11" ht="15" customHeight="1">
       <c r="B151" s="18" t="s">
         <v>125</v>
       </c>
@@ -3949,8 +3996,12 @@
       <c r="D151" s="7"/>
       <c r="E151" s="29"/>
       <c r="G151" s="21"/>
-    </row>
-    <row r="152" spans="2:8" ht="15" customHeight="1">
+      <c r="I151" s="6" cm="1">
+        <f t="array" aca="1" ref="I151" ca="1">ABS(COLUMN(INDIRECT(I150))-COLUMN(INDIRECT("S9")))</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="2:11" ht="15" customHeight="1">
       <c r="B152" s="18" t="s">
         <v>97</v>
       </c>
@@ -3958,8 +4009,12 @@
       <c r="D152" s="7"/>
       <c r="E152" s="29"/>
       <c r="G152" s="21"/>
-    </row>
-    <row r="153" spans="2:8" ht="15" customHeight="1" thickBot="1">
+      <c r="I152" s="6" cm="1">
+        <f t="array" aca="1" ref="I152" ca="1">ABS(ROW(INDIRECT(I150))-ROW(INDIRECT("S9")))</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B153" s="18" t="s">
         <v>205</v>
       </c>
@@ -3967,8 +4022,12 @@
       <c r="D153" s="7"/>
       <c r="E153" s="29"/>
       <c r="G153" s="21"/>
-    </row>
-    <row r="154" spans="2:8" ht="25.2" customHeight="1" thickBot="1">
+      <c r="I153" s="6">
+        <f ca="1">SQRT(I151^2+I152^2)</f>
+        <v>12.529964086141668</v>
+      </c>
+    </row>
+    <row r="154" spans="2:11" ht="25.2" customHeight="1" thickBot="1">
       <c r="B154" s="1" t="s">
         <v>2</v>
       </c>
@@ -3985,12 +4044,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="155" spans="2:8">
+    <row r="155" spans="2:11">
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="6"/>
     </row>
-    <row r="156" spans="2:8" ht="23.4">
+    <row r="156" spans="2:11" ht="23.4" customHeight="1">
       <c r="B156" s="15" t="s">
         <v>16</v>
       </c>
@@ -4007,13 +4066,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="157" spans="2:8">
+    <row r="157" spans="2:11" ht="23.4" customHeight="1">
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="E157" s="22"/>
-    </row>
-    <row r="158" spans="2:8" ht="23.25" customHeight="1">
+      <c r="J157" s="6">
+        <f ca="1">I153</f>
+        <v>12.529964086141668</v>
+      </c>
+    </row>
+    <row r="158" spans="2:11" ht="23.25" customHeight="1">
       <c r="B158" s="15">
         <v>51</v>
       </c>
@@ -4023,13 +4086,27 @@
       <c r="D158" s="23">
         <v>7</v>
       </c>
-      <c r="E158" s="5"/>
+      <c r="E158" s="5">
+        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(G158&amp;":S9"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>15</v>
+      </c>
       <c r="G158" s="24" t="s">
         <v>90</v>
       </c>
       <c r="H158" s="20"/>
-    </row>
-    <row r="159" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I158" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="J158" s="6">
+        <f t="dataTable" ref="J158:J177" dt2D="0" dtr="0" r1="I150" ca="1"/>
+        <v>15.297058540778355</v>
+      </c>
+      <c r="K158" s="6" cm="1">
+        <f t="array" ref="K158:K177">{15;12;17;15;11;21;16;10;2;5;15;15;10;20;11;11;12;11;6;13}</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="159" spans="2:11" ht="23.25" customHeight="1">
       <c r="B159" s="15">
         <v>52</v>
       </c>
@@ -4039,13 +4116,25 @@
       <c r="D159" s="23">
         <v>7</v>
       </c>
-      <c r="E159" s="5"/>
+      <c r="E159" s="5">
+        <f t="shared" ref="E159:E177" ca="1" si="0">_xlfn.LET(_xlpm.range,INDIRECT(G159&amp;":S9"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>12</v>
+      </c>
       <c r="G159" s="24" t="s">
         <v>100</v>
       </c>
       <c r="H159" s="20"/>
-    </row>
-    <row r="160" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I159" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="J159" s="6">
+        <v>12</v>
+      </c>
+      <c r="K159" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="160" spans="2:11" ht="23.25" customHeight="1">
       <c r="B160" s="15">
         <v>53</v>
       </c>
@@ -4055,13 +4144,25 @@
       <c r="D160" s="23">
         <v>7</v>
       </c>
-      <c r="E160" s="5"/>
+      <c r="E160" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>17</v>
+      </c>
       <c r="G160" s="24" t="s">
         <v>101</v>
       </c>
       <c r="H160" s="20"/>
-    </row>
-    <row r="161" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I160" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J160" s="6">
+        <v>17</v>
+      </c>
+      <c r="K160" s="6">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="2:11" ht="23.25" customHeight="1">
       <c r="B161" s="15">
         <v>54</v>
       </c>
@@ -4071,13 +4172,25 @@
       <c r="D161" s="23">
         <v>7</v>
       </c>
-      <c r="E161" s="5"/>
+      <c r="E161" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
       <c r="G161" s="24" t="s">
         <v>102</v>
       </c>
       <c r="H161" s="20"/>
-    </row>
-    <row r="162" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I161" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J161" s="6">
+        <v>15.524174696260024</v>
+      </c>
+      <c r="K161" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="162" spans="2:11" ht="23.25" customHeight="1">
       <c r="B162" s="15">
         <v>55</v>
       </c>
@@ -4087,13 +4200,25 @@
       <c r="D162" s="23">
         <v>7</v>
       </c>
-      <c r="E162" s="5"/>
+      <c r="E162" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
       <c r="G162" s="24" t="s">
         <v>103</v>
       </c>
       <c r="H162" s="20"/>
-    </row>
-    <row r="163" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I162" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="J162" s="6">
+        <v>12.529964086141668</v>
+      </c>
+      <c r="K162" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="2:11" ht="23.25" customHeight="1">
       <c r="B163" s="15">
         <v>56</v>
       </c>
@@ -4103,13 +4228,25 @@
       <c r="D163" s="23">
         <v>7</v>
       </c>
-      <c r="E163" s="5"/>
+      <c r="E163" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>21</v>
+      </c>
       <c r="G163" s="24" t="s">
         <v>104</v>
       </c>
       <c r="H163" s="20"/>
-    </row>
-    <row r="164" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I163" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="J163" s="6">
+        <v>21</v>
+      </c>
+      <c r="K163" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="164" spans="2:11" ht="23.25" customHeight="1">
       <c r="B164" s="15">
         <v>57</v>
       </c>
@@ -4119,13 +4256,25 @@
       <c r="D164" s="23">
         <v>7</v>
       </c>
-      <c r="E164" s="5"/>
+      <c r="E164" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
       <c r="G164" s="24" t="s">
         <v>105</v>
       </c>
       <c r="H164" s="20"/>
-    </row>
-    <row r="165" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I164" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J164" s="6">
+        <v>16.492422502470642</v>
+      </c>
+      <c r="K164" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="165" spans="2:11" ht="23.25" customHeight="1">
       <c r="B165" s="15">
         <v>58</v>
       </c>
@@ -4135,13 +4284,25 @@
       <c r="D165" s="23">
         <v>7</v>
       </c>
-      <c r="E165" s="5"/>
+      <c r="E165" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
       <c r="G165" s="24" t="s">
         <v>106</v>
       </c>
       <c r="H165" s="20"/>
-    </row>
-    <row r="166" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I165" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="J165" s="6">
+        <v>10.770329614269007</v>
+      </c>
+      <c r="K165" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="2:11" ht="23.25" customHeight="1">
       <c r="B166" s="15">
         <v>59</v>
       </c>
@@ -4151,13 +4312,25 @@
       <c r="D166" s="23">
         <v>7</v>
       </c>
-      <c r="E166" s="5"/>
+      <c r="E166" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
       <c r="G166" s="24" t="s">
         <v>107</v>
       </c>
       <c r="H166" s="20"/>
-    </row>
-    <row r="167" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I166" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J166" s="6">
+        <v>2.8284271247461903</v>
+      </c>
+      <c r="K166" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="2:11" ht="23.25" customHeight="1">
       <c r="B167" s="15">
         <v>60</v>
       </c>
@@ -4167,13 +4340,25 @@
       <c r="D167" s="23">
         <v>7</v>
       </c>
-      <c r="E167" s="5"/>
+      <c r="E167" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
       <c r="G167" s="24" t="s">
         <v>108</v>
       </c>
       <c r="H167" s="20"/>
-    </row>
-    <row r="168" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I167" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="J167" s="6">
+        <v>6.4031242374328485</v>
+      </c>
+      <c r="K167" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="168" spans="2:11" ht="23.25" customHeight="1">
       <c r="B168" s="15">
         <v>61</v>
       </c>
@@ -4183,13 +4368,25 @@
       <c r="D168" s="23">
         <v>7</v>
       </c>
-      <c r="E168" s="5"/>
+      <c r="E168" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
       <c r="G168" s="24" t="s">
         <v>109</v>
       </c>
       <c r="H168" s="20"/>
-    </row>
-    <row r="169" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I168" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J168" s="6">
+        <v>15.132745950421556</v>
+      </c>
+      <c r="K168" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="169" spans="2:11" ht="23.25" customHeight="1">
       <c r="B169" s="15">
         <v>62</v>
       </c>
@@ -4199,13 +4396,25 @@
       <c r="D169" s="23">
         <v>7</v>
       </c>
-      <c r="E169" s="5"/>
+      <c r="E169" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>15</v>
+      </c>
       <c r="G169" s="24" t="s">
         <v>110</v>
       </c>
       <c r="H169" s="20"/>
-    </row>
-    <row r="170" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I169" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="J169" s="6">
+        <v>17</v>
+      </c>
+      <c r="K169" s="6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="170" spans="2:11" ht="23.25" customHeight="1">
       <c r="B170" s="15">
         <v>63</v>
       </c>
@@ -4215,13 +4424,25 @@
       <c r="D170" s="23">
         <v>7</v>
       </c>
-      <c r="E170" s="5"/>
+      <c r="E170" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
       <c r="G170" s="24" t="s">
         <v>111</v>
       </c>
       <c r="H170" s="20"/>
-    </row>
-    <row r="171" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I170" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J170" s="6">
+        <v>12.206555615733702</v>
+      </c>
+      <c r="K170" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="2:11" ht="23.25" customHeight="1">
       <c r="B171" s="15">
         <v>64</v>
       </c>
@@ -4231,13 +4452,25 @@
       <c r="D171" s="23">
         <v>7</v>
       </c>
-      <c r="E171" s="5"/>
+      <c r="E171" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>20</v>
+      </c>
       <c r="G171" s="24" t="s">
         <v>112</v>
       </c>
       <c r="H171" s="20"/>
-    </row>
-    <row r="172" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I171" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J171" s="6">
+        <v>20.024984394500787</v>
+      </c>
+      <c r="K171" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="172" spans="2:11" ht="23.25" customHeight="1">
       <c r="B172" s="15">
         <v>65</v>
       </c>
@@ -4247,13 +4480,25 @@
       <c r="D172" s="23">
         <v>7</v>
       </c>
-      <c r="E172" s="5"/>
+      <c r="E172" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
       <c r="G172" s="24" t="s">
         <v>113</v>
       </c>
       <c r="H172" s="20"/>
-    </row>
-    <row r="173" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I172" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="J172" s="6">
+        <v>15.556349186104045</v>
+      </c>
+      <c r="K172" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="2:11" ht="23.25" customHeight="1">
       <c r="B173" s="15">
         <v>66</v>
       </c>
@@ -4263,13 +4508,25 @@
       <c r="D173" s="23">
         <v>7</v>
       </c>
-      <c r="E173" s="5"/>
+      <c r="E173" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
       <c r="G173" s="24" t="s">
         <v>114</v>
       </c>
       <c r="H173" s="20"/>
-    </row>
-    <row r="174" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I173" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J173" s="6">
+        <v>14.212670403551895</v>
+      </c>
+      <c r="K173" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="174" spans="2:11" ht="23.25" customHeight="1">
       <c r="B174" s="15">
         <v>67</v>
       </c>
@@ -4279,13 +4536,25 @@
       <c r="D174" s="23">
         <v>7</v>
       </c>
-      <c r="E174" s="5"/>
+      <c r="E174" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>12</v>
+      </c>
       <c r="G174" s="24" t="s">
         <v>89</v>
       </c>
       <c r="H174" s="20"/>
-    </row>
-    <row r="175" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I174" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="J174" s="6">
+        <v>12.649110640673518</v>
+      </c>
+      <c r="K174" s="6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="175" spans="2:11" ht="23.25" customHeight="1">
       <c r="B175" s="15">
         <v>68</v>
       </c>
@@ -4295,13 +4564,25 @@
       <c r="D175" s="23">
         <v>7</v>
       </c>
-      <c r="E175" s="5"/>
+      <c r="E175" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
       <c r="G175" s="24" t="s">
         <v>115</v>
       </c>
       <c r="H175" s="20"/>
-    </row>
-    <row r="176" spans="2:8" ht="23.25" customHeight="1">
+      <c r="I175" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="J175" s="6">
+        <v>13.601470508735444</v>
+      </c>
+      <c r="K175" s="6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="176" spans="2:11" ht="23.25" customHeight="1">
       <c r="B176" s="15">
         <v>69</v>
       </c>
@@ -4311,11 +4592,23 @@
       <c r="D176" s="23">
         <v>7</v>
       </c>
-      <c r="E176" s="5"/>
+      <c r="E176" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
       <c r="G176" s="24" t="s">
         <v>116</v>
       </c>
       <c r="H176" s="20"/>
+      <c r="I176" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="J176" s="6">
+        <v>6.0827625302982193</v>
+      </c>
+      <c r="K176" s="6">
+        <v>6</v>
+      </c>
     </row>
     <row r="177" spans="1:11" ht="23.25" customHeight="1">
       <c r="B177" s="15">
@@ -4327,11 +4620,23 @@
       <c r="D177" s="23">
         <v>7</v>
       </c>
-      <c r="E177" s="5"/>
+      <c r="E177" s="5">
+        <f t="shared" ca="1" si="0"/>
+        <v>13</v>
+      </c>
       <c r="G177" s="24" t="s">
         <v>84</v>
       </c>
       <c r="H177" s="20"/>
+      <c r="I177" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J177" s="6">
+        <v>13.601470508735444</v>
+      </c>
+      <c r="K177" s="6">
+        <v>13</v>
+      </c>
     </row>
     <row r="178" spans="1:11">
       <c r="B178" s="7"/>
@@ -4351,8 +4656,8 @@
         <v>0</v>
       </c>
       <c r="E179" s="37" t="str">
-        <f>_xlfn.TEXTJOIN(";",FALSE,E158:E177)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <f ca="1">_xlfn.TEXTJOIN(";",FALSE,E158:E177)</f>
+        <v>15;12;17;15;11;21;16;10;2;5;15;15;10;20;11;11;12;11;6;13</v>
       </c>
     </row>
     <row r="180" spans="1:11" ht="15" thickBot="1">

</xml_diff>

<commit_message>
Problems 1-5 now done
</commit_message>
<xml_diff>
--- a/The_Maps_Case.xlsx
+++ b/The_Maps_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74973EAC-1F9C-4944-81D5-AB91336990B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAEB423-A8C1-4983-867B-55B070745929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <definedName name="_m">Map_Copy!$B$2:$AQ$30</definedName>
     <definedName name="_map">The_Map_for_the_Training_Case!$B$2:$AQ$30</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="210">
   <si>
     <t>Case Author</t>
   </si>
@@ -724,8 +724,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1339,17 +1339,17 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1368,17 +1368,17 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
@@ -1428,6 +1428,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1474,9 +1477,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2015,8 +2015,8 @@
   </sheetPr>
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A212" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G223" sqref="G223"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C183" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E221" sqref="E221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -2036,17 +2036,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="33.6" customHeight="1">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="76" t="s">
         <v>195</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="76"/>
+      <c r="J1" s="76"/>
     </row>
     <row r="2" spans="2:11" ht="33.6" customHeight="1">
       <c r="B2" s="9"/>
@@ -2060,10 +2060,10 @@
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:11" ht="33.6" customHeight="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="75"/>
+      <c r="C3" s="76"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -2073,10 +2073,10 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="2:11" ht="33.6" customHeight="1">
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="76"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -2096,120 +2096,120 @@
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:11" ht="21.75" customHeight="1">
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="74"/>
-      <c r="D7" s="74"/>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
-      <c r="I7" s="74"/>
-      <c r="J7" s="85"/>
+      <c r="C7" s="75"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
+      <c r="I7" s="75"/>
+      <c r="J7" s="86"/>
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="2:11" ht="14.25" customHeight="1">
-      <c r="B8" s="76" t="s">
+      <c r="B8" s="77" t="s">
         <v>196</v>
       </c>
-      <c r="C8" s="77"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
-      <c r="I8" s="77"/>
-      <c r="J8" s="78"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="78"/>
+      <c r="E8" s="78"/>
+      <c r="F8" s="78"/>
+      <c r="G8" s="78"/>
+      <c r="H8" s="78"/>
+      <c r="I8" s="78"/>
+      <c r="J8" s="79"/>
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B9" s="79"/>
-      <c r="C9" s="80"/>
-      <c r="D9" s="80"/>
-      <c r="E9" s="80"/>
-      <c r="F9" s="80"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="80"/>
-      <c r="J9" s="81"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="82"/>
     </row>
     <row r="10" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B10" s="79"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="81"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="81"/>
+      <c r="D10" s="81"/>
+      <c r="E10" s="81"/>
+      <c r="F10" s="81"/>
+      <c r="G10" s="81"/>
+      <c r="H10" s="81"/>
+      <c r="I10" s="81"/>
+      <c r="J10" s="82"/>
     </row>
     <row r="11" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B11" s="79"/>
-      <c r="C11" s="80"/>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="81"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="81"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
+      <c r="F11" s="81"/>
+      <c r="G11" s="81"/>
+      <c r="H11" s="81"/>
+      <c r="I11" s="81"/>
+      <c r="J11" s="82"/>
     </row>
     <row r="12" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B12" s="79"/>
-      <c r="C12" s="80"/>
-      <c r="D12" s="80"/>
-      <c r="E12" s="80"/>
-      <c r="F12" s="80"/>
-      <c r="G12" s="80"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="80"/>
-      <c r="J12" s="81"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="81"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="81"/>
+      <c r="I12" s="81"/>
+      <c r="J12" s="82"/>
     </row>
     <row r="13" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B13" s="79"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="80"/>
-      <c r="H13" s="80"/>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
+      <c r="B13" s="80"/>
+      <c r="C13" s="81"/>
+      <c r="D13" s="81"/>
+      <c r="E13" s="81"/>
+      <c r="F13" s="81"/>
+      <c r="G13" s="81"/>
+      <c r="H13" s="81"/>
+      <c r="I13" s="81"/>
+      <c r="J13" s="82"/>
     </row>
     <row r="14" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B14" s="79"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="80"/>
-      <c r="J14" s="81"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="81"/>
+      <c r="D14" s="81"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="81"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="82"/>
     </row>
     <row r="15" spans="2:11" ht="21.75" customHeight="1">
-      <c r="B15" s="79"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="81"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="81"/>
+      <c r="D15" s="81"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="81"/>
+      <c r="G15" s="81"/>
+      <c r="H15" s="81"/>
+      <c r="I15" s="81"/>
+      <c r="J15" s="82"/>
     </row>
     <row r="16" spans="2:11" ht="21.75" customHeight="1">
-      <c r="B16" s="82"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="83"/>
-      <c r="E16" s="83"/>
-      <c r="F16" s="83"/>
-      <c r="G16" s="83"/>
-      <c r="H16" s="83"/>
-      <c r="I16" s="83"/>
-      <c r="J16" s="84"/>
+      <c r="B16" s="83"/>
+      <c r="C16" s="84"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="84"/>
+      <c r="G16" s="84"/>
+      <c r="H16" s="84"/>
+      <c r="I16" s="84"/>
+      <c r="J16" s="85"/>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1">
@@ -2220,18 +2220,18 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:11" ht="21">
-      <c r="B18" s="73" t="s">
+      <c r="B18" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="74"/>
-      <c r="D18" s="74"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
+      <c r="C18" s="75"/>
+      <c r="D18" s="75"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
+      <c r="J18" s="75"/>
+      <c r="K18" s="75"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B19" s="16"/>
@@ -3481,7 +3481,7 @@
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
-      <c r="E118" s="87" cm="1">
+      <c r="E118" s="71" cm="1">
         <f t="array" aca="1" ref="E118" ca="1">_xlfn.LET(_xlpm.c, ABS(COLUMN(INDIRECT(G118))-COLUMN(INDIRECT("S1"))),_xlpm.r,ABS(ROW(INDIRECT(G118))-9),_xlpm.r+_xlpm.c)</f>
         <v>1</v>
       </c>
@@ -4700,67 +4700,82 @@
     </row>
     <row r="184" spans="1:11" ht="15" customHeight="1">
       <c r="A184" s="7"/>
-      <c r="B184" s="71" t="s">
+      <c r="B184" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="C184" s="71"/>
-      <c r="D184" s="71"/>
-      <c r="E184" s="71"/>
-      <c r="F184" s="71"/>
-      <c r="G184" s="71"/>
+      <c r="C184" s="72"/>
+      <c r="D184" s="72"/>
+      <c r="E184" s="72"/>
+      <c r="F184" s="72"/>
+      <c r="G184" s="72"/>
       <c r="J184" s="30"/>
       <c r="K184" s="30"/>
     </row>
     <row r="185" spans="1:11" ht="15" customHeight="1">
       <c r="A185" s="7"/>
-      <c r="B185" s="71"/>
-      <c r="C185" s="71"/>
-      <c r="D185" s="71"/>
-      <c r="E185" s="71"/>
-      <c r="F185" s="71"/>
-      <c r="G185" s="71"/>
+      <c r="B185" s="72"/>
+      <c r="C185" s="72"/>
+      <c r="D185" s="72"/>
+      <c r="E185" s="72"/>
+      <c r="F185" s="72"/>
+      <c r="G185" s="72"/>
+      <c r="H185" s="6" t="s">
+        <v>135</v>
+      </c>
       <c r="J185" s="30"/>
       <c r="K185" s="30"/>
     </row>
     <row r="186" spans="1:11" ht="15" customHeight="1" thickBot="1">
       <c r="A186" s="7"/>
-      <c r="B186" s="71"/>
-      <c r="C186" s="71"/>
-      <c r="D186" s="71"/>
-      <c r="E186" s="71"/>
-      <c r="F186" s="71"/>
-      <c r="G186" s="71"/>
+      <c r="B186" s="72"/>
+      <c r="C186" s="72"/>
+      <c r="D186" s="72"/>
+      <c r="E186" s="72"/>
+      <c r="F186" s="72"/>
+      <c r="G186" s="72"/>
       <c r="J186" s="30"/>
       <c r="K186" s="30"/>
     </row>
     <row r="187" spans="1:11" ht="15" customHeight="1">
       <c r="A187" s="7"/>
-      <c r="B187" s="71"/>
-      <c r="C187" s="71"/>
-      <c r="D187" s="71"/>
-      <c r="E187" s="71"/>
-      <c r="F187" s="71"/>
-      <c r="G187" s="71"/>
+      <c r="B187" s="72"/>
+      <c r="C187" s="72"/>
+      <c r="D187" s="72"/>
+      <c r="E187" s="72"/>
+      <c r="F187" s="72"/>
+      <c r="G187" s="72"/>
       <c r="H187" s="63" t="s">
         <v>132</v>
       </c>
       <c r="J187" s="30"/>
-      <c r="K187" s="30"/>
+      <c r="K187" s="30">
+        <f ca="1">MIN(K188:K193)</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="188" spans="1:11" ht="15" customHeight="1">
       <c r="A188" s="7"/>
-      <c r="B188" s="71"/>
-      <c r="C188" s="71"/>
-      <c r="D188" s="71"/>
-      <c r="E188" s="71"/>
-      <c r="F188" s="71"/>
-      <c r="G188" s="71"/>
+      <c r="B188" s="72"/>
+      <c r="C188" s="72"/>
+      <c r="D188" s="72"/>
+      <c r="E188" s="72"/>
+      <c r="F188" s="72"/>
+      <c r="G188" s="72"/>
       <c r="H188" s="64" t="s">
         <v>90</v>
       </c>
-      <c r="I188" s="7"/>
-      <c r="J188" s="30"/>
-      <c r="K188" s="30"/>
+      <c r="I188" s="7">
+        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT($H$185&amp;":"&amp;H188),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>23</v>
+      </c>
+      <c r="J188" s="30">
+        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(H188&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>12</v>
+      </c>
+      <c r="K188" s="30">
+        <f ca="1">I188+J188</f>
+        <v>35</v>
+      </c>
     </row>
     <row r="189" spans="1:11" ht="15" customHeight="1">
       <c r="A189" s="7"/>
@@ -4775,9 +4790,18 @@
       <c r="H189" s="65" t="s">
         <v>100</v>
       </c>
-      <c r="I189" s="7"/>
-      <c r="J189" s="30"/>
-      <c r="K189" s="30"/>
+      <c r="I189" s="7">
+        <f t="shared" ref="I189:I193" ca="1" si="1">_xlfn.LET(_xlpm.range,INDIRECT($H$185&amp;":"&amp;H189),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>16</v>
+      </c>
+      <c r="J189" s="30">
+        <f t="shared" ref="J189:J194" ca="1" si="2">_xlfn.LET(_xlpm.range,INDIRECT(H189&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>15</v>
+      </c>
+      <c r="K189" s="30">
+        <f t="shared" ref="K189:K194" ca="1" si="3">I189+J189</f>
+        <v>31</v>
+      </c>
     </row>
     <row r="190" spans="1:11" ht="15" customHeight="1">
       <c r="A190" s="7"/>
@@ -4790,9 +4814,18 @@
       <c r="H190" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="I190" s="7"/>
-      <c r="J190" s="30"/>
-      <c r="K190" s="30"/>
+      <c r="I190" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="J190" s="30">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="K190" s="30">
+        <f t="shared" ca="1" si="3"/>
+        <v>21</v>
+      </c>
     </row>
     <row r="191" spans="1:11" ht="15" customHeight="1">
       <c r="B191" s="18" t="s">
@@ -4805,8 +4838,18 @@
       <c r="H191" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="I191" s="31"/>
-      <c r="J191" s="31"/>
+      <c r="I191" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="J191" s="30">
+        <f t="shared" ca="1" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="K191" s="30">
+        <f t="shared" ca="1" si="3"/>
+        <v>39</v>
+      </c>
     </row>
     <row r="192" spans="1:11" ht="15" customHeight="1">
       <c r="B192" s="19" t="s">
@@ -4819,8 +4862,18 @@
       <c r="H192" s="65" t="s">
         <v>102</v>
       </c>
-      <c r="I192" s="31"/>
-      <c r="J192" s="31"/>
+      <c r="I192" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="J192" s="30">
+        <f t="shared" ca="1" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="K192" s="30">
+        <f t="shared" ca="1" si="3"/>
+        <v>35</v>
+      </c>
     </row>
     <row r="193" spans="2:11" ht="15" customHeight="1">
       <c r="B193" s="19" t="s">
@@ -4833,8 +4886,18 @@
       <c r="H193" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="I193" s="31"/>
-      <c r="J193" s="31"/>
+      <c r="I193" s="7">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J193" s="30">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="K193" s="30">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="194" spans="2:11" ht="15" customHeight="1">
       <c r="B194" s="27" t="s">
@@ -4846,7 +4909,8 @@
       <c r="G194" s="31"/>
       <c r="H194" s="7"/>
       <c r="I194" s="31"/>
-      <c r="J194" s="31"/>
+      <c r="J194" s="30"/>
+      <c r="K194" s="30"/>
     </row>
     <row r="195" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B195" s="27"/>
@@ -4888,7 +4952,7 @@
       <c r="J197" s="20"/>
       <c r="K197" s="20"/>
     </row>
-    <row r="198" spans="2:11" ht="23.4">
+    <row r="198" spans="2:11" ht="23.4" customHeight="1">
       <c r="B198" s="15" t="s">
         <v>18</v>
       </c>
@@ -4904,19 +4968,25 @@
       <c r="G198" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="H198" s="7"/>
+      <c r="H198" s="7">
+        <f ca="1">K187</f>
+        <v>14</v>
+      </c>
       <c r="I198" s="20"/>
       <c r="J198" s="20"/>
       <c r="K198" s="20"/>
     </row>
-    <row r="199" spans="2:11">
+    <row r="199" spans="2:11" ht="23.4" customHeight="1">
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="6"/>
       <c r="G199" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H199" s="7"/>
+        <v>135</v>
+      </c>
+      <c r="H199" s="7">
+        <f t="dataTable" ref="H199:H219" dt2D="0" dtr="0" r1="H185" ca="1"/>
+        <v>14</v>
+      </c>
       <c r="I199" s="20"/>
       <c r="J199" s="20"/>
       <c r="K199" s="20"/>
@@ -4931,11 +5001,15 @@
       <c r="D200" s="23">
         <v>8</v>
       </c>
-      <c r="E200" s="5"/>
+      <c r="E200" s="5">
+        <v>14</v>
+      </c>
       <c r="G200" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="H200" s="7"/>
+      <c r="H200" s="7">
+        <v>7</v>
+      </c>
       <c r="I200" s="20"/>
       <c r="J200" s="20"/>
       <c r="K200" s="20"/>
@@ -4950,11 +5024,15 @@
       <c r="D201" s="23">
         <v>8</v>
       </c>
-      <c r="E201" s="5"/>
+      <c r="E201" s="5">
+        <v>7</v>
+      </c>
       <c r="G201" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="H201" s="20"/>
+      <c r="H201" s="20">
+        <v>8</v>
+      </c>
       <c r="I201" s="20"/>
       <c r="J201" s="20"/>
       <c r="K201" s="20"/>
@@ -4969,11 +5047,15 @@
       <c r="D202" s="23">
         <v>8</v>
       </c>
-      <c r="E202" s="5"/>
+      <c r="E202" s="5">
+        <v>8</v>
+      </c>
       <c r="G202" s="24" t="s">
         <v>144</v>
       </c>
-      <c r="H202" s="20"/>
+      <c r="H202" s="20">
+        <v>10</v>
+      </c>
       <c r="I202" s="20"/>
       <c r="J202" s="20"/>
       <c r="K202" s="20"/>
@@ -4988,11 +5070,15 @@
       <c r="D203" s="23">
         <v>8</v>
       </c>
-      <c r="E203" s="5"/>
+      <c r="E203" s="5">
+        <v>10</v>
+      </c>
       <c r="G203" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="H203" s="20"/>
+      <c r="H203" s="20">
+        <v>15</v>
+      </c>
       <c r="I203" s="20"/>
       <c r="J203" s="20"/>
       <c r="K203" s="20"/>
@@ -5007,11 +5093,15 @@
       <c r="D204" s="23">
         <v>8</v>
       </c>
-      <c r="E204" s="5"/>
+      <c r="E204" s="5">
+        <v>15</v>
+      </c>
       <c r="G204" s="24" t="s">
         <v>146</v>
       </c>
-      <c r="H204" s="20"/>
+      <c r="H204" s="20">
+        <v>20</v>
+      </c>
       <c r="I204" s="20"/>
       <c r="J204" s="20"/>
       <c r="K204" s="20"/>
@@ -5026,11 +5116,15 @@
       <c r="D205" s="23">
         <v>8</v>
       </c>
-      <c r="E205" s="5"/>
+      <c r="E205" s="5">
+        <v>20</v>
+      </c>
       <c r="G205" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="H205" s="20"/>
+      <c r="H205" s="20">
+        <v>7</v>
+      </c>
       <c r="I205" s="20"/>
       <c r="J205" s="20"/>
       <c r="K205" s="20"/>
@@ -5045,11 +5139,15 @@
       <c r="D206" s="23">
         <v>8</v>
       </c>
-      <c r="E206" s="5"/>
+      <c r="E206" s="5">
+        <v>7</v>
+      </c>
       <c r="G206" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="H206" s="20"/>
+      <c r="H206" s="20">
+        <v>14</v>
+      </c>
       <c r="I206" s="20"/>
       <c r="J206" s="20"/>
       <c r="K206" s="20"/>
@@ -5064,11 +5162,15 @@
       <c r="D207" s="23">
         <v>8</v>
       </c>
-      <c r="E207" s="5"/>
+      <c r="E207" s="5">
+        <v>14</v>
+      </c>
       <c r="G207" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="H207" s="20"/>
+      <c r="H207" s="20">
+        <v>14</v>
+      </c>
       <c r="I207" s="20"/>
       <c r="J207" s="20"/>
       <c r="K207" s="20"/>
@@ -5083,11 +5185,15 @@
       <c r="D208" s="23">
         <v>8</v>
       </c>
-      <c r="E208" s="5"/>
+      <c r="E208" s="5">
+        <v>14</v>
+      </c>
       <c r="G208" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="H208" s="20"/>
+      <c r="H208" s="20">
+        <v>11</v>
+      </c>
       <c r="I208" s="20"/>
       <c r="J208" s="20"/>
       <c r="K208" s="20"/>
@@ -5102,11 +5208,15 @@
       <c r="D209" s="23">
         <v>8</v>
       </c>
-      <c r="E209" s="5"/>
+      <c r="E209" s="5">
+        <v>11</v>
+      </c>
       <c r="G209" s="24" t="s">
         <v>148</v>
       </c>
-      <c r="H209" s="20"/>
+      <c r="H209" s="20">
+        <v>16</v>
+      </c>
       <c r="I209" s="20"/>
       <c r="J209" s="20"/>
       <c r="K209" s="20"/>
@@ -5121,11 +5231,15 @@
       <c r="D210" s="23">
         <v>8</v>
       </c>
-      <c r="E210" s="5"/>
+      <c r="E210" s="5">
+        <v>16</v>
+      </c>
       <c r="G210" s="24" t="s">
         <v>149</v>
       </c>
-      <c r="H210" s="20"/>
+      <c r="H210" s="20">
+        <v>17</v>
+      </c>
       <c r="I210" s="20"/>
       <c r="J210" s="20"/>
       <c r="K210" s="20"/>
@@ -5140,11 +5254,15 @@
       <c r="D211" s="23">
         <v>8</v>
       </c>
-      <c r="E211" s="5"/>
+      <c r="E211" s="5">
+        <v>17</v>
+      </c>
       <c r="G211" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="H211" s="20"/>
+      <c r="H211" s="20">
+        <v>13</v>
+      </c>
       <c r="I211" s="20"/>
       <c r="J211" s="20"/>
       <c r="K211" s="20"/>
@@ -5159,11 +5277,15 @@
       <c r="D212" s="23">
         <v>8</v>
       </c>
-      <c r="E212" s="5"/>
+      <c r="E212" s="5">
+        <v>13</v>
+      </c>
       <c r="G212" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="H212" s="20"/>
+      <c r="H212" s="20">
+        <v>16</v>
+      </c>
       <c r="I212" s="20"/>
       <c r="J212" s="20"/>
       <c r="K212" s="20"/>
@@ -5178,11 +5300,15 @@
       <c r="D213" s="23">
         <v>8</v>
       </c>
-      <c r="E213" s="5"/>
+      <c r="E213" s="5">
+        <v>16</v>
+      </c>
       <c r="G213" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="H213" s="20"/>
+      <c r="H213" s="20">
+        <v>15</v>
+      </c>
       <c r="I213" s="20"/>
       <c r="J213" s="20"/>
       <c r="K213" s="20"/>
@@ -5197,11 +5323,15 @@
       <c r="D214" s="23">
         <v>8</v>
       </c>
-      <c r="E214" s="5"/>
+      <c r="E214" s="5">
+        <v>15</v>
+      </c>
       <c r="G214" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="H214" s="20"/>
+      <c r="H214" s="20">
+        <v>16</v>
+      </c>
       <c r="I214" s="20"/>
       <c r="J214" s="20"/>
       <c r="K214" s="20"/>
@@ -5216,11 +5346,15 @@
       <c r="D215" s="23">
         <v>8</v>
       </c>
-      <c r="E215" s="5"/>
+      <c r="E215" s="5">
+        <v>16</v>
+      </c>
       <c r="G215" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="H215" s="20"/>
+      <c r="H215" s="20">
+        <v>16</v>
+      </c>
       <c r="I215" s="20"/>
       <c r="J215" s="20"/>
       <c r="K215" s="20"/>
@@ -5235,11 +5369,15 @@
       <c r="D216" s="23">
         <v>8</v>
       </c>
-      <c r="E216" s="5"/>
+      <c r="E216" s="5">
+        <v>16</v>
+      </c>
       <c r="G216" s="24" t="s">
         <v>152</v>
       </c>
-      <c r="H216" s="20"/>
+      <c r="H216" s="20">
+        <v>19</v>
+      </c>
       <c r="I216" s="20"/>
       <c r="J216" s="20"/>
       <c r="K216" s="20"/>
@@ -5254,11 +5392,15 @@
       <c r="D217" s="23">
         <v>8</v>
       </c>
-      <c r="E217" s="5"/>
+      <c r="E217" s="5">
+        <v>19</v>
+      </c>
       <c r="G217" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="H217" s="20"/>
+      <c r="H217" s="20">
+        <v>18</v>
+      </c>
       <c r="I217" s="20"/>
       <c r="J217" s="20"/>
       <c r="K217" s="20"/>
@@ -5273,11 +5415,15 @@
       <c r="D218" s="23">
         <v>8</v>
       </c>
-      <c r="E218" s="5"/>
+      <c r="E218" s="5">
+        <v>18</v>
+      </c>
       <c r="G218" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="H218" s="20"/>
+      <c r="H218" s="20">
+        <v>14</v>
+      </c>
       <c r="I218" s="20"/>
       <c r="J218" s="20"/>
       <c r="K218" s="20"/>
@@ -5292,17 +5438,23 @@
       <c r="D219" s="23">
         <v>8</v>
       </c>
-      <c r="E219" s="5"/>
+      <c r="E219" s="5">
+        <v>14</v>
+      </c>
       <c r="G219" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="H219" s="20"/>
+      <c r="H219" s="20">
+        <v>16</v>
+      </c>
       <c r="I219" s="20"/>
       <c r="J219" s="20"/>
       <c r="K219" s="20"/>
     </row>
     <row r="220" spans="2:11" ht="15" customHeight="1">
-      <c r="E220" s="12"/>
+      <c r="E220" s="12">
+        <v>16</v>
+      </c>
     </row>
     <row r="221" spans="2:11" ht="31.2">
       <c r="B221" s="15" t="s">
@@ -5317,7 +5469,7 @@
       </c>
       <c r="E221" s="37" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E200:E219)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <v>14;7;8;10;15;20;7;14;14;11;16;17;13;16;15;16;16;19;18;14</v>
       </c>
     </row>
     <row r="222" spans="2:11" ht="15" customHeight="1" thickBot="1">
@@ -5353,41 +5505,41 @@
     </row>
     <row r="226" spans="1:9" ht="15" customHeight="1">
       <c r="A226" s="7"/>
-      <c r="B226" s="72" t="s">
+      <c r="B226" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="C226" s="72"/>
-      <c r="D226" s="72"/>
-      <c r="E226" s="72"/>
-      <c r="F226" s="72"/>
-      <c r="G226" s="72"/>
+      <c r="C226" s="73"/>
+      <c r="D226" s="73"/>
+      <c r="E226" s="73"/>
+      <c r="F226" s="73"/>
+      <c r="G226" s="73"/>
     </row>
     <row r="227" spans="1:9" ht="15" customHeight="1">
       <c r="A227" s="7"/>
-      <c r="B227" s="72"/>
-      <c r="C227" s="72"/>
-      <c r="D227" s="72"/>
-      <c r="E227" s="72"/>
-      <c r="F227" s="72"/>
-      <c r="G227" s="72"/>
+      <c r="B227" s="73"/>
+      <c r="C227" s="73"/>
+      <c r="D227" s="73"/>
+      <c r="E227" s="73"/>
+      <c r="F227" s="73"/>
+      <c r="G227" s="73"/>
     </row>
     <row r="228" spans="1:9" ht="15" customHeight="1">
       <c r="A228" s="7"/>
-      <c r="B228" s="72"/>
-      <c r="C228" s="72"/>
-      <c r="D228" s="72"/>
-      <c r="E228" s="72"/>
-      <c r="F228" s="72"/>
-      <c r="G228" s="72"/>
+      <c r="B228" s="73"/>
+      <c r="C228" s="73"/>
+      <c r="D228" s="73"/>
+      <c r="E228" s="73"/>
+      <c r="F228" s="73"/>
+      <c r="G228" s="73"/>
     </row>
     <row r="229" spans="1:9" ht="15" customHeight="1">
       <c r="A229" s="7"/>
-      <c r="B229" s="72"/>
-      <c r="C229" s="72"/>
-      <c r="D229" s="72"/>
-      <c r="E229" s="72"/>
-      <c r="F229" s="72"/>
-      <c r="G229" s="72"/>
+      <c r="B229" s="73"/>
+      <c r="C229" s="73"/>
+      <c r="D229" s="73"/>
+      <c r="E229" s="73"/>
+      <c r="F229" s="73"/>
+      <c r="G229" s="73"/>
     </row>
     <row r="230" spans="1:9" ht="15" customHeight="1">
       <c r="B230" s="19"/>
@@ -7450,10 +7602,10 @@
       <c r="AO13" s="49"/>
       <c r="AP13" s="49"/>
       <c r="AQ13" s="50"/>
-      <c r="AZ13" s="86" t="s">
+      <c r="AZ13" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="BA13" s="86"/>
+      <c r="BA13" s="87"/>
     </row>
     <row r="14" spans="1:75">
       <c r="A14">
@@ -9465,10 +9617,10 @@
       <c r="AO13" s="49"/>
       <c r="AP13" s="49"/>
       <c r="AQ13" s="50"/>
-      <c r="AZ13" s="86" t="s">
+      <c r="AZ13" s="87" t="s">
         <v>62</v>
       </c>
-      <c r="BA13" s="86"/>
+      <c r="BA13" s="87"/>
     </row>
     <row r="14" spans="1:75">
       <c r="A14">
@@ -10649,48 +10801,48 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
+      <c r="B6" s="72"/>
+      <c r="C6" s="72"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="72"/>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="72"/>
+      <c r="G8" s="72"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
+      <c r="B9" s="72"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="18" t="s">

</xml_diff>

<commit_message>
Found a problem with #5
</commit_message>
<xml_diff>
--- a/The_Maps_Case.xlsx
+++ b/The_Maps_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAEB423-A8C1-4983-867B-55B070745929}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B2EBC5-E42E-4066-AD85-690E50F1690B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
+    <workbookView xWindow="3180" yWindow="1488" windowWidth="17280" windowHeight="8880" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="211">
   <si>
     <t>Case Author</t>
   </si>
@@ -716,6 +716,9 @@
   </si>
   <si>
     <t>What is the Quickest Time Possible while staying on the road? (you travel at the same speed as Hanna; 1 cell = 1 minute)</t>
+  </si>
+  <si>
+    <t>k25</t>
   </si>
 </sst>
 </file>
@@ -2015,8 +2018,8 @@
   </sheetPr>
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C183" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E221" sqref="E221"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F199" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H200" sqref="H200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -4023,8 +4026,8 @@
       <c r="E153" s="29"/>
       <c r="G153" s="21"/>
       <c r="I153" s="6">
-        <f ca="1">SQRT(I151^2+I152^2)</f>
-        <v>12.529964086141668</v>
+        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(I150&amp;":S9"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>11</v>
       </c>
     </row>
     <row r="154" spans="2:11" ht="25.2" customHeight="1" thickBot="1">
@@ -4073,7 +4076,7 @@
       <c r="E157" s="22"/>
       <c r="J157" s="6">
         <f ca="1">I153</f>
-        <v>12.529964086141668</v>
+        <v>11</v>
       </c>
     </row>
     <row r="158" spans="2:11" ht="23.25" customHeight="1">
@@ -4087,7 +4090,6 @@
         <v>7</v>
       </c>
       <c r="E158" s="5">
-        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(G158&amp;":S9"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
         <v>15</v>
       </c>
       <c r="G158" s="24" t="s">
@@ -4099,7 +4101,7 @@
       </c>
       <c r="J158" s="6">
         <f t="dataTable" ref="J158:J177" dt2D="0" dtr="0" r1="I150" ca="1"/>
-        <v>15.297058540778355</v>
+        <v>15</v>
       </c>
       <c r="K158" s="6" cm="1">
         <f t="array" ref="K158:K177">{15;12;17;15;11;21;16;10;2;5;15;15;10;20;11;11;12;11;6;13}</f>
@@ -4117,7 +4119,6 @@
         <v>7</v>
       </c>
       <c r="E159" s="5">
-        <f t="shared" ref="E159:E177" ca="1" si="0">_xlfn.LET(_xlpm.range,INDIRECT(G159&amp;":S9"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
         <v>12</v>
       </c>
       <c r="G159" s="24" t="s">
@@ -4145,7 +4146,6 @@
         <v>7</v>
       </c>
       <c r="E160" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>17</v>
       </c>
       <c r="G160" s="24" t="s">
@@ -4173,7 +4173,6 @@
         <v>7</v>
       </c>
       <c r="E161" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="G161" s="24" t="s">
@@ -4184,7 +4183,7 @@
         <v>102</v>
       </c>
       <c r="J161" s="6">
-        <v>15.524174696260024</v>
+        <v>15</v>
       </c>
       <c r="K161" s="6">
         <v>15</v>
@@ -4201,7 +4200,6 @@
         <v>7</v>
       </c>
       <c r="E162" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="G162" s="24" t="s">
@@ -4212,7 +4210,7 @@
         <v>103</v>
       </c>
       <c r="J162" s="6">
-        <v>12.529964086141668</v>
+        <v>11</v>
       </c>
       <c r="K162" s="6">
         <v>11</v>
@@ -4229,7 +4227,6 @@
         <v>7</v>
       </c>
       <c r="E163" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>21</v>
       </c>
       <c r="G163" s="24" t="s">
@@ -4257,7 +4254,6 @@
         <v>7</v>
       </c>
       <c r="E164" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>16</v>
       </c>
       <c r="G164" s="24" t="s">
@@ -4268,7 +4264,7 @@
         <v>105</v>
       </c>
       <c r="J164" s="6">
-        <v>16.492422502470642</v>
+        <v>16</v>
       </c>
       <c r="K164" s="6">
         <v>16</v>
@@ -4285,7 +4281,6 @@
         <v>7</v>
       </c>
       <c r="E165" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="G165" s="24" t="s">
@@ -4296,7 +4291,7 @@
         <v>106</v>
       </c>
       <c r="J165" s="6">
-        <v>10.770329614269007</v>
+        <v>10</v>
       </c>
       <c r="K165" s="6">
         <v>10</v>
@@ -4313,7 +4308,6 @@
         <v>7</v>
       </c>
       <c r="E166" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>2</v>
       </c>
       <c r="G166" s="24" t="s">
@@ -4324,7 +4318,7 @@
         <v>107</v>
       </c>
       <c r="J166" s="6">
-        <v>2.8284271247461903</v>
+        <v>2</v>
       </c>
       <c r="K166" s="6">
         <v>2</v>
@@ -4341,7 +4335,6 @@
         <v>7</v>
       </c>
       <c r="E167" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="G167" s="24" t="s">
@@ -4352,7 +4345,7 @@
         <v>108</v>
       </c>
       <c r="J167" s="6">
-        <v>6.4031242374328485</v>
+        <v>5</v>
       </c>
       <c r="K167" s="6">
         <v>5</v>
@@ -4369,7 +4362,6 @@
         <v>7</v>
       </c>
       <c r="E168" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="G168" s="24" t="s">
@@ -4380,7 +4372,7 @@
         <v>109</v>
       </c>
       <c r="J168" s="6">
-        <v>15.132745950421556</v>
+        <v>15</v>
       </c>
       <c r="K168" s="6">
         <v>15</v>
@@ -4397,7 +4389,6 @@
         <v>7</v>
       </c>
       <c r="E169" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>15</v>
       </c>
       <c r="G169" s="24" t="s">
@@ -4408,7 +4399,7 @@
         <v>110</v>
       </c>
       <c r="J169" s="6">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K169" s="6">
         <v>15</v>
@@ -4425,7 +4416,6 @@
         <v>7</v>
       </c>
       <c r="E170" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="G170" s="24" t="s">
@@ -4436,7 +4426,7 @@
         <v>111</v>
       </c>
       <c r="J170" s="6">
-        <v>12.206555615733702</v>
+        <v>10</v>
       </c>
       <c r="K170" s="6">
         <v>10</v>
@@ -4453,7 +4443,6 @@
         <v>7</v>
       </c>
       <c r="E171" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>20</v>
       </c>
       <c r="G171" s="24" t="s">
@@ -4464,7 +4453,7 @@
         <v>112</v>
       </c>
       <c r="J171" s="6">
-        <v>20.024984394500787</v>
+        <v>20</v>
       </c>
       <c r="K171" s="6">
         <v>20</v>
@@ -4481,7 +4470,6 @@
         <v>7</v>
       </c>
       <c r="E172" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="G172" s="24" t="s">
@@ -4492,7 +4480,7 @@
         <v>113</v>
       </c>
       <c r="J172" s="6">
-        <v>15.556349186104045</v>
+        <v>11</v>
       </c>
       <c r="K172" s="6">
         <v>11</v>
@@ -4509,7 +4497,6 @@
         <v>7</v>
       </c>
       <c r="E173" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="G173" s="24" t="s">
@@ -4520,7 +4507,7 @@
         <v>114</v>
       </c>
       <c r="J173" s="6">
-        <v>14.212670403551895</v>
+        <v>11</v>
       </c>
       <c r="K173" s="6">
         <v>11</v>
@@ -4537,7 +4524,6 @@
         <v>7</v>
       </c>
       <c r="E174" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>12</v>
       </c>
       <c r="G174" s="24" t="s">
@@ -4548,7 +4534,7 @@
         <v>89</v>
       </c>
       <c r="J174" s="6">
-        <v>12.649110640673518</v>
+        <v>12</v>
       </c>
       <c r="K174" s="6">
         <v>12</v>
@@ -4565,7 +4551,6 @@
         <v>7</v>
       </c>
       <c r="E175" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>11</v>
       </c>
       <c r="G175" s="24" t="s">
@@ -4576,7 +4561,7 @@
         <v>115</v>
       </c>
       <c r="J175" s="6">
-        <v>13.601470508735444</v>
+        <v>11</v>
       </c>
       <c r="K175" s="6">
         <v>11</v>
@@ -4593,7 +4578,6 @@
         <v>7</v>
       </c>
       <c r="E176" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="G176" s="24" t="s">
@@ -4604,7 +4588,7 @@
         <v>116</v>
       </c>
       <c r="J176" s="6">
-        <v>6.0827625302982193</v>
+        <v>6</v>
       </c>
       <c r="K176" s="6">
         <v>6</v>
@@ -4621,7 +4605,6 @@
         <v>7</v>
       </c>
       <c r="E177" s="5">
-        <f t="shared" ca="1" si="0"/>
         <v>13</v>
       </c>
       <c r="G177" s="24" t="s">
@@ -4632,7 +4615,7 @@
         <v>84</v>
       </c>
       <c r="J177" s="6">
-        <v>13.601470508735444</v>
+        <v>13</v>
       </c>
       <c r="K177" s="6">
         <v>13</v>
@@ -4656,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="E179" s="37" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(";",FALSE,E158:E177)</f>
+        <f>_xlfn.TEXTJOIN(";",FALSE,E158:E177)</f>
         <v>15;12;17;15;11;21;16;10;2;5;15;15;10;20;11;11;12;11;6;13</v>
       </c>
     </row>
@@ -4720,7 +4703,7 @@
       <c r="F185" s="72"/>
       <c r="G185" s="72"/>
       <c r="H185" s="6" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="J185" s="30"/>
       <c r="K185" s="30"/>
@@ -4748,10 +4731,7 @@
         <v>132</v>
       </c>
       <c r="J187" s="30"/>
-      <c r="K187" s="30">
-        <f ca="1">MIN(K188:K193)</f>
-        <v>14</v>
-      </c>
+      <c r="K187" s="30"/>
     </row>
     <row r="188" spans="1:11" ht="15" customHeight="1">
       <c r="A188" s="7"/>
@@ -4769,13 +4749,10 @@
         <v>23</v>
       </c>
       <c r="J188" s="30">
-        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(H188&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
-        <v>12</v>
-      </c>
-      <c r="K188" s="30">
-        <f ca="1">I188+J188</f>
-        <v>35</v>
-      </c>
+        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(H188&amp;":V14"),MAX(ROWS(_xlpm.range),COLUMNS(_xlpm.range)))</f>
+        <v>13</v>
+      </c>
+      <c r="K188" s="30"/>
     </row>
     <row r="189" spans="1:11" ht="15" customHeight="1">
       <c r="A189" s="7"/>
@@ -4791,17 +4768,14 @@
         <v>100</v>
       </c>
       <c r="I189" s="7">
-        <f t="shared" ref="I189:I193" ca="1" si="1">_xlfn.LET(_xlpm.range,INDIRECT($H$185&amp;":"&amp;H189),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <f t="shared" ref="I189:I193" ca="1" si="0">_xlfn.LET(_xlpm.range,INDIRECT($H$185&amp;":"&amp;H189),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
         <v>16</v>
       </c>
       <c r="J189" s="30">
-        <f t="shared" ref="J189:J194" ca="1" si="2">_xlfn.LET(_xlpm.range,INDIRECT(H189&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <f t="shared" ref="J189:J194" ca="1" si="1">_xlfn.LET(_xlpm.range,INDIRECT(H189&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
         <v>15</v>
       </c>
-      <c r="K189" s="30">
-        <f t="shared" ref="K189:K194" ca="1" si="3">I189+J189</f>
-        <v>31</v>
-      </c>
+      <c r="K189" s="30"/>
     </row>
     <row r="190" spans="1:11" ht="15" customHeight="1">
       <c r="A190" s="7"/>
@@ -4815,17 +4789,14 @@
         <v>73</v>
       </c>
       <c r="I190" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="J190" s="30">
         <f t="shared" ca="1" si="1"/>
-        <v>16</v>
-      </c>
-      <c r="J190" s="30">
-        <f t="shared" ca="1" si="2"/>
         <v>5</v>
       </c>
-      <c r="K190" s="30">
-        <f t="shared" ca="1" si="3"/>
-        <v>21</v>
-      </c>
+      <c r="K190" s="30"/>
     </row>
     <row r="191" spans="1:11" ht="15" customHeight="1">
       <c r="B191" s="18" t="s">
@@ -4839,17 +4810,14 @@
         <v>101</v>
       </c>
       <c r="I191" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="J191" s="30">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
-      </c>
-      <c r="J191" s="30">
-        <f t="shared" ca="1" si="2"/>
         <v>14</v>
       </c>
-      <c r="K191" s="30">
-        <f t="shared" ca="1" si="3"/>
-        <v>39</v>
-      </c>
+      <c r="K191" s="30"/>
     </row>
     <row r="192" spans="1:11" ht="15" customHeight="1">
       <c r="B192" s="19" t="s">
@@ -4863,17 +4831,14 @@
         <v>102</v>
       </c>
       <c r="I192" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J192" s="30">
         <f t="shared" ca="1" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="J192" s="30">
-        <f t="shared" ca="1" si="2"/>
         <v>12</v>
       </c>
-      <c r="K192" s="30">
-        <f t="shared" ca="1" si="3"/>
-        <v>35</v>
-      </c>
+      <c r="K192" s="30"/>
     </row>
     <row r="193" spans="2:11" ht="15" customHeight="1">
       <c r="B193" s="19" t="s">
@@ -4887,17 +4852,14 @@
         <v>103</v>
       </c>
       <c r="I193" s="7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J193" s="30">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="J193" s="30">
-        <f t="shared" ca="1" si="2"/>
         <v>9</v>
       </c>
-      <c r="K193" s="30">
-        <f t="shared" ca="1" si="3"/>
-        <v>14</v>
-      </c>
+      <c r="K193" s="30"/>
     </row>
     <row r="194" spans="2:11" ht="15" customHeight="1">
       <c r="B194" s="27" t="s">
@@ -4907,10 +4869,22 @@
       <c r="D194" s="31"/>
       <c r="E194" s="32"/>
       <c r="G194" s="31"/>
-      <c r="H194" s="7"/>
-      <c r="I194" s="31"/>
-      <c r="J194" s="30"/>
-      <c r="K194" s="30"/>
+      <c r="H194" s="7" t="str">
+        <f ca="1">_xlfn.XLOOKUP(I194,I188:I193,H188:H193)</f>
+        <v>M20</v>
+      </c>
+      <c r="I194" s="31">
+        <f ca="1">MIN(I188:I193)</f>
+        <v>5</v>
+      </c>
+      <c r="J194" s="30">
+        <f ca="1">_xlfn.LET(_xlpm.range,INDIRECT(H194&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <v>9</v>
+      </c>
+      <c r="K194" s="30">
+        <f t="shared" ref="K189:K194" ca="1" si="2">I194+J194</f>
+        <v>14</v>
+      </c>
     </row>
     <row r="195" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B195" s="27"/>
@@ -4969,7 +4943,7 @@
         <v>135</v>
       </c>
       <c r="H198" s="7">
-        <f ca="1">K187</f>
+        <f ca="1">K194</f>
         <v>14</v>
       </c>
       <c r="I198" s="20"/>
@@ -4984,7 +4958,7 @@
         <v>135</v>
       </c>
       <c r="H199" s="7">
-        <f t="dataTable" ref="H199:H219" dt2D="0" dtr="0" r1="H185" ca="1"/>
+        <f ca="1">K194</f>
         <v>14</v>
       </c>
       <c r="I199" s="20"/>
@@ -5002,15 +4976,19 @@
         <v>8</v>
       </c>
       <c r="E200" s="5">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G200" s="24" t="s">
         <v>142</v>
       </c>
       <c r="H200" s="7">
+        <f t="dataTable" ref="H200:H219" dt2D="0" dtr="0" r1="H185" ca="1"/>
         <v>7</v>
       </c>
-      <c r="I200" s="20"/>
+      <c r="I200" s="20" cm="1">
+        <f t="array" ref="I200:I219">{7;8;10;15;21;7;14;14;11;16;20;13;22;20;20;17;19;18;14;17}</f>
+        <v>7</v>
+      </c>
       <c r="J200" s="20"/>
       <c r="K200" s="20"/>
     </row>
@@ -5025,7 +5003,7 @@
         <v>8</v>
       </c>
       <c r="E201" s="5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G201" s="24" t="s">
         <v>143</v>
@@ -5033,7 +5011,9 @@
       <c r="H201" s="20">
         <v>8</v>
       </c>
-      <c r="I201" s="20"/>
+      <c r="I201" s="20">
+        <v>8</v>
+      </c>
       <c r="J201" s="20"/>
       <c r="K201" s="20"/>
     </row>
@@ -5048,7 +5028,7 @@
         <v>8</v>
       </c>
       <c r="E202" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G202" s="24" t="s">
         <v>144</v>
@@ -5056,7 +5036,9 @@
       <c r="H202" s="20">
         <v>10</v>
       </c>
-      <c r="I202" s="20"/>
+      <c r="I202" s="20">
+        <v>10</v>
+      </c>
       <c r="J202" s="20"/>
       <c r="K202" s="20"/>
     </row>
@@ -5071,7 +5053,7 @@
         <v>8</v>
       </c>
       <c r="E203" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="G203" s="24" t="s">
         <v>145</v>
@@ -5079,7 +5061,9 @@
       <c r="H203" s="20">
         <v>15</v>
       </c>
-      <c r="I203" s="20"/>
+      <c r="I203" s="20">
+        <v>15</v>
+      </c>
       <c r="J203" s="20"/>
       <c r="K203" s="20"/>
     </row>
@@ -5094,15 +5078,17 @@
         <v>8</v>
       </c>
       <c r="E204" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G204" s="24" t="s">
         <v>146</v>
       </c>
       <c r="H204" s="20">
-        <v>20</v>
-      </c>
-      <c r="I204" s="20"/>
+        <v>21</v>
+      </c>
+      <c r="I204" s="20">
+        <v>21</v>
+      </c>
       <c r="J204" s="20"/>
       <c r="K204" s="20"/>
     </row>
@@ -5117,7 +5103,7 @@
         <v>8</v>
       </c>
       <c r="E205" s="5">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G205" s="24" t="s">
         <v>136</v>
@@ -5125,7 +5111,9 @@
       <c r="H205" s="20">
         <v>7</v>
       </c>
-      <c r="I205" s="20"/>
+      <c r="I205" s="20">
+        <v>7</v>
+      </c>
       <c r="J205" s="20"/>
       <c r="K205" s="20"/>
     </row>
@@ -5140,7 +5128,7 @@
         <v>8</v>
       </c>
       <c r="E206" s="5">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="G206" s="24" t="s">
         <v>147</v>
@@ -5148,7 +5136,9 @@
       <c r="H206" s="20">
         <v>14</v>
       </c>
-      <c r="I206" s="20"/>
+      <c r="I206" s="20">
+        <v>14</v>
+      </c>
       <c r="J206" s="20"/>
       <c r="K206" s="20"/>
     </row>
@@ -5171,7 +5161,9 @@
       <c r="H207" s="20">
         <v>14</v>
       </c>
-      <c r="I207" s="20"/>
+      <c r="I207" s="20">
+        <v>14</v>
+      </c>
       <c r="J207" s="20"/>
       <c r="K207" s="20"/>
     </row>
@@ -5186,7 +5178,7 @@
         <v>8</v>
       </c>
       <c r="E208" s="5">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G208" s="24" t="s">
         <v>138</v>
@@ -5194,7 +5186,9 @@
       <c r="H208" s="20">
         <v>11</v>
       </c>
-      <c r="I208" s="20"/>
+      <c r="I208" s="20">
+        <v>11</v>
+      </c>
       <c r="J208" s="20"/>
       <c r="K208" s="20"/>
     </row>
@@ -5209,7 +5203,7 @@
         <v>8</v>
       </c>
       <c r="E209" s="5">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G209" s="24" t="s">
         <v>148</v>
@@ -5217,7 +5211,9 @@
       <c r="H209" s="20">
         <v>16</v>
       </c>
-      <c r="I209" s="20"/>
+      <c r="I209" s="20">
+        <v>16</v>
+      </c>
       <c r="J209" s="20"/>
       <c r="K209" s="20"/>
     </row>
@@ -5232,15 +5228,17 @@
         <v>8</v>
       </c>
       <c r="E210" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G210" s="24" t="s">
         <v>149</v>
       </c>
       <c r="H210" s="20">
-        <v>17</v>
-      </c>
-      <c r="I210" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="I210" s="20">
+        <v>20</v>
+      </c>
       <c r="J210" s="20"/>
       <c r="K210" s="20"/>
     </row>
@@ -5255,7 +5253,7 @@
         <v>8</v>
       </c>
       <c r="E211" s="5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="G211" s="24" t="s">
         <v>139</v>
@@ -5263,7 +5261,9 @@
       <c r="H211" s="20">
         <v>13</v>
       </c>
-      <c r="I211" s="20"/>
+      <c r="I211" s="20">
+        <v>13</v>
+      </c>
       <c r="J211" s="20"/>
       <c r="K211" s="20"/>
     </row>
@@ -5278,15 +5278,17 @@
         <v>8</v>
       </c>
       <c r="E212" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G212" s="24" t="s">
         <v>150</v>
       </c>
       <c r="H212" s="20">
-        <v>16</v>
-      </c>
-      <c r="I212" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="I212" s="20">
+        <v>22</v>
+      </c>
       <c r="J212" s="20"/>
       <c r="K212" s="20"/>
     </row>
@@ -5301,15 +5303,17 @@
         <v>8</v>
       </c>
       <c r="E213" s="5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G213" s="24" t="s">
         <v>111</v>
       </c>
       <c r="H213" s="20">
-        <v>15</v>
-      </c>
-      <c r="I213" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="I213" s="20">
+        <v>20</v>
+      </c>
       <c r="J213" s="20"/>
       <c r="K213" s="20"/>
     </row>
@@ -5324,15 +5328,17 @@
         <v>8</v>
       </c>
       <c r="E214" s="5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G214" s="24" t="s">
         <v>151</v>
       </c>
       <c r="H214" s="20">
-        <v>16</v>
-      </c>
-      <c r="I214" s="20"/>
+        <v>20</v>
+      </c>
+      <c r="I214" s="20">
+        <v>20</v>
+      </c>
       <c r="J214" s="20"/>
       <c r="K214" s="20"/>
     </row>
@@ -5353,9 +5359,11 @@
         <v>157</v>
       </c>
       <c r="H215" s="20">
-        <v>16</v>
-      </c>
-      <c r="I215" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="I215" s="20">
+        <v>17</v>
+      </c>
       <c r="J215" s="20"/>
       <c r="K215" s="20"/>
     </row>
@@ -5370,7 +5378,7 @@
         <v>8</v>
       </c>
       <c r="E216" s="5">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G216" s="24" t="s">
         <v>152</v>
@@ -5378,7 +5386,9 @@
       <c r="H216" s="20">
         <v>19</v>
       </c>
-      <c r="I216" s="20"/>
+      <c r="I216" s="20">
+        <v>19</v>
+      </c>
       <c r="J216" s="20"/>
       <c r="K216" s="20"/>
     </row>
@@ -5393,7 +5403,7 @@
         <v>8</v>
       </c>
       <c r="E217" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G217" s="24" t="s">
         <v>153</v>
@@ -5401,7 +5411,9 @@
       <c r="H217" s="20">
         <v>18</v>
       </c>
-      <c r="I217" s="20"/>
+      <c r="I217" s="20">
+        <v>18</v>
+      </c>
       <c r="J217" s="20"/>
       <c r="K217" s="20"/>
     </row>
@@ -5416,7 +5428,7 @@
         <v>8</v>
       </c>
       <c r="E218" s="5">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G218" s="24" t="s">
         <v>158</v>
@@ -5424,7 +5436,9 @@
       <c r="H218" s="20">
         <v>14</v>
       </c>
-      <c r="I218" s="20"/>
+      <c r="I218" s="20">
+        <v>14</v>
+      </c>
       <c r="J218" s="20"/>
       <c r="K218" s="20"/>
     </row>
@@ -5439,22 +5453,22 @@
         <v>8</v>
       </c>
       <c r="E219" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G219" s="24" t="s">
         <v>140</v>
       </c>
       <c r="H219" s="20">
-        <v>16</v>
-      </c>
-      <c r="I219" s="20"/>
+        <v>17</v>
+      </c>
+      <c r="I219" s="20">
+        <v>17</v>
+      </c>
       <c r="J219" s="20"/>
       <c r="K219" s="20"/>
     </row>
     <row r="220" spans="2:11" ht="15" customHeight="1">
-      <c r="E220" s="12">
-        <v>16</v>
-      </c>
+      <c r="E220" s="12"/>
     </row>
     <row r="221" spans="2:11" ht="31.2">
       <c r="B221" s="15" t="s">
@@ -5469,7 +5483,7 @@
       </c>
       <c r="E221" s="37" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E200:E219)</f>
-        <v>14;7;8;10;15;20;7;14;14;11;16;17;13;16;15;16;16;19;18;14</v>
+        <v>7;8;10;15;20;7;14;14;11;16;17;13;16;15;16;16;19;18;14;16</v>
       </c>
     </row>
     <row r="222" spans="2:11" ht="15" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
Found another problem with #5
</commit_message>
<xml_diff>
--- a/The_Maps_Case.xlsx
+++ b/The_Maps_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B2EBC5-E42E-4066-AD85-690E50F1690B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E995E87-9398-4DEF-8449-1DD0CA1E36DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1488" windowWidth="17280" windowHeight="8880" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
@@ -2018,8 +2018,8 @@
   </sheetPr>
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F199" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H200" sqref="H200"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A197" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E200" sqref="E200:E219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -4772,7 +4772,7 @@
         <v>16</v>
       </c>
       <c r="J189" s="30">
-        <f t="shared" ref="J189:J194" ca="1" si="1">_xlfn.LET(_xlpm.range,INDIRECT(H189&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
+        <f t="shared" ref="J189:J193" ca="1" si="1">_xlfn.LET(_xlpm.range,INDIRECT(H189&amp;":V14"),MAX(ROWS(_xlpm.range)-1,COLUMNS(_xlpm.range)-1))</f>
         <v>15</v>
       </c>
       <c r="K189" s="30"/>
@@ -4882,7 +4882,7 @@
         <v>9</v>
       </c>
       <c r="K194" s="30">
-        <f t="shared" ref="K189:K194" ca="1" si="2">I194+J194</f>
+        <f t="shared" ref="K194" ca="1" si="2">I194+J194</f>
         <v>14</v>
       </c>
     </row>
@@ -5078,7 +5078,7 @@
         <v>8</v>
       </c>
       <c r="E204" s="5">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G204" s="24" t="s">
         <v>146</v>
@@ -5228,7 +5228,7 @@
         <v>8</v>
       </c>
       <c r="E210" s="5">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G210" s="24" t="s">
         <v>149</v>
@@ -5278,7 +5278,7 @@
         <v>8</v>
       </c>
       <c r="E212" s="5">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G212" s="24" t="s">
         <v>150</v>
@@ -5303,7 +5303,7 @@
         <v>8</v>
       </c>
       <c r="E213" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G213" s="24" t="s">
         <v>111</v>
@@ -5328,7 +5328,7 @@
         <v>8</v>
       </c>
       <c r="E214" s="5">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="G214" s="24" t="s">
         <v>151</v>
@@ -5353,7 +5353,7 @@
         <v>8</v>
       </c>
       <c r="E215" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G215" s="24" t="s">
         <v>157</v>
@@ -5453,7 +5453,7 @@
         <v>8</v>
       </c>
       <c r="E219" s="5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G219" s="24" t="s">
         <v>140</v>
@@ -5483,7 +5483,7 @@
       </c>
       <c r="E221" s="37" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E200:E219)</f>
-        <v>7;8;10;15;20;7;14;14;11;16;17;13;16;15;16;16;19;18;14;16</v>
+        <v>7;8;10;15;21;7;14;14;11;16;20;13;22;20;20;17;19;18;14;17</v>
       </c>
     </row>
     <row r="222" spans="2:11" ht="15" customHeight="1" thickBot="1">

</xml_diff>

<commit_message>
All answered. I need to look at Case 7 in more detail
</commit_message>
<xml_diff>
--- a/The_Maps_Case.xlsx
+++ b/The_Maps_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F43AB8-8B0E-4440-9440-FD7C816E1650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D6B0B6-F4CF-48A0-9B79-6A5C1A4A2B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_m">Map_Copy!$B$2:$AQ$30</definedName>
     <definedName name="_map">The_Map_for_the_Training_Case!$B$2:$AQ$30</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1302,7 +1302,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1453,6 +1453,8 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1501,8 +1503,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -2039,8 +2042,8 @@
   </sheetPr>
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A265" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G277" sqref="G277"/>
+    <sheetView showGridLines="0" topLeftCell="A275" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H283" sqref="H283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -2060,17 +2063,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="33.6" customHeight="1">
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="78" t="s">
         <v>194</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
+      <c r="G1" s="78"/>
+      <c r="H1" s="78"/>
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
     </row>
     <row r="2" spans="2:11" ht="33.6" customHeight="1">
       <c r="B2" s="9"/>
@@ -2084,10 +2087,10 @@
       <c r="J2" s="9"/>
     </row>
     <row r="3" spans="2:11" ht="33.6" customHeight="1">
-      <c r="B3" s="76" t="s">
+      <c r="B3" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="76"/>
+      <c r="C3" s="78"/>
       <c r="D3" s="9"/>
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
@@ -2097,10 +2100,10 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="2:11" ht="33.6" customHeight="1">
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="76"/>
+      <c r="C4" s="78"/>
       <c r="D4" s="9"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
@@ -2120,120 +2123,120 @@
       <c r="D6" s="9"/>
     </row>
     <row r="7" spans="2:11" ht="21.75" customHeight="1">
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="75"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
-      <c r="I7" s="75"/>
-      <c r="J7" s="86"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="77"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="77"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="77"/>
+      <c r="I7" s="77"/>
+      <c r="J7" s="88"/>
       <c r="K7" s="11"/>
     </row>
     <row r="8" spans="2:11" ht="14.25" customHeight="1">
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="79" t="s">
         <v>195</v>
       </c>
-      <c r="C8" s="78"/>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
-      <c r="F8" s="78"/>
-      <c r="G8" s="78"/>
-      <c r="H8" s="78"/>
-      <c r="I8" s="78"/>
-      <c r="J8" s="79"/>
+      <c r="C8" s="80"/>
+      <c r="D8" s="80"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="80"/>
+      <c r="H8" s="80"/>
+      <c r="I8" s="80"/>
+      <c r="J8" s="81"/>
       <c r="K8" s="11"/>
     </row>
     <row r="9" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="82"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="83"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="84"/>
     </row>
     <row r="10" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B10" s="80"/>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="82"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="83"/>
+      <c r="D10" s="83"/>
+      <c r="E10" s="83"/>
+      <c r="F10" s="83"/>
+      <c r="G10" s="83"/>
+      <c r="H10" s="83"/>
+      <c r="I10" s="83"/>
+      <c r="J10" s="84"/>
     </row>
     <row r="11" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B11" s="80"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="81"/>
-      <c r="E11" s="81"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="81"/>
-      <c r="H11" s="81"/>
-      <c r="I11" s="81"/>
-      <c r="J11" s="82"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="83"/>
+      <c r="D11" s="83"/>
+      <c r="E11" s="83"/>
+      <c r="F11" s="83"/>
+      <c r="G11" s="83"/>
+      <c r="H11" s="83"/>
+      <c r="I11" s="83"/>
+      <c r="J11" s="84"/>
     </row>
     <row r="12" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B12" s="80"/>
-      <c r="C12" s="81"/>
-      <c r="D12" s="81"/>
-      <c r="E12" s="81"/>
-      <c r="F12" s="81"/>
-      <c r="G12" s="81"/>
-      <c r="H12" s="81"/>
-      <c r="I12" s="81"/>
-      <c r="J12" s="82"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="83"/>
+      <c r="D12" s="83"/>
+      <c r="E12" s="83"/>
+      <c r="F12" s="83"/>
+      <c r="G12" s="83"/>
+      <c r="H12" s="83"/>
+      <c r="I12" s="83"/>
+      <c r="J12" s="84"/>
     </row>
     <row r="13" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B13" s="80"/>
-      <c r="C13" s="81"/>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="81"/>
-      <c r="I13" s="81"/>
-      <c r="J13" s="82"/>
+      <c r="B13" s="82"/>
+      <c r="C13" s="83"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="83"/>
+      <c r="F13" s="83"/>
+      <c r="G13" s="83"/>
+      <c r="H13" s="83"/>
+      <c r="I13" s="83"/>
+      <c r="J13" s="84"/>
     </row>
     <row r="14" spans="2:11" ht="21.9" customHeight="1">
-      <c r="B14" s="80"/>
-      <c r="C14" s="81"/>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="81"/>
-      <c r="I14" s="81"/>
-      <c r="J14" s="82"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="83"/>
+      <c r="D14" s="83"/>
+      <c r="E14" s="83"/>
+      <c r="F14" s="83"/>
+      <c r="G14" s="83"/>
+      <c r="H14" s="83"/>
+      <c r="I14" s="83"/>
+      <c r="J14" s="84"/>
     </row>
     <row r="15" spans="2:11" ht="21.75" customHeight="1">
-      <c r="B15" s="80"/>
-      <c r="C15" s="81"/>
-      <c r="D15" s="81"/>
-      <c r="E15" s="81"/>
-      <c r="F15" s="81"/>
-      <c r="G15" s="81"/>
-      <c r="H15" s="81"/>
-      <c r="I15" s="81"/>
-      <c r="J15" s="82"/>
+      <c r="B15" s="82"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="84"/>
     </row>
     <row r="16" spans="2:11" ht="21.75" customHeight="1">
-      <c r="B16" s="83"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="85"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="87"/>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="2:11" ht="15" customHeight="1">
@@ -2244,18 +2247,18 @@
       <c r="F17" s="6"/>
     </row>
     <row r="18" spans="2:11" ht="21">
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="75"/>
-      <c r="D18" s="75"/>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
-      <c r="I18" s="75"/>
-      <c r="J18" s="75"/>
-      <c r="K18" s="75"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
+      <c r="I18" s="77"/>
+      <c r="J18" s="77"/>
+      <c r="K18" s="77"/>
     </row>
     <row r="19" spans="2:11" ht="15" customHeight="1" thickBot="1">
       <c r="B19" s="16"/>
@@ -4704,25 +4707,25 @@
     </row>
     <row r="184" spans="1:11" ht="15" customHeight="1">
       <c r="A184" s="7"/>
-      <c r="B184" s="72" t="s">
+      <c r="B184" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="C184" s="72"/>
-      <c r="D184" s="72"/>
-      <c r="E184" s="72"/>
-      <c r="F184" s="72"/>
-      <c r="G184" s="72"/>
+      <c r="C184" s="74"/>
+      <c r="D184" s="74"/>
+      <c r="E184" s="74"/>
+      <c r="F184" s="74"/>
+      <c r="G184" s="74"/>
       <c r="J184" s="30"/>
       <c r="K184" s="30"/>
     </row>
     <row r="185" spans="1:11" ht="15" customHeight="1">
       <c r="A185" s="7"/>
-      <c r="B185" s="72"/>
-      <c r="C185" s="72"/>
-      <c r="D185" s="72"/>
-      <c r="E185" s="72"/>
-      <c r="F185" s="72"/>
-      <c r="G185" s="72"/>
+      <c r="B185" s="74"/>
+      <c r="C185" s="74"/>
+      <c r="D185" s="74"/>
+      <c r="E185" s="74"/>
+      <c r="F185" s="74"/>
+      <c r="G185" s="74"/>
       <c r="H185" s="6" t="s">
         <v>209</v>
       </c>
@@ -4731,23 +4734,23 @@
     </row>
     <row r="186" spans="1:11" ht="15" customHeight="1" thickBot="1">
       <c r="A186" s="7"/>
-      <c r="B186" s="72"/>
-      <c r="C186" s="72"/>
-      <c r="D186" s="72"/>
-      <c r="E186" s="72"/>
-      <c r="F186" s="72"/>
-      <c r="G186" s="72"/>
+      <c r="B186" s="74"/>
+      <c r="C186" s="74"/>
+      <c r="D186" s="74"/>
+      <c r="E186" s="74"/>
+      <c r="F186" s="74"/>
+      <c r="G186" s="74"/>
       <c r="J186" s="30"/>
       <c r="K186" s="30"/>
     </row>
     <row r="187" spans="1:11" ht="15" customHeight="1">
       <c r="A187" s="7"/>
-      <c r="B187" s="72"/>
-      <c r="C187" s="72"/>
-      <c r="D187" s="72"/>
-      <c r="E187" s="72"/>
-      <c r="F187" s="72"/>
-      <c r="G187" s="72"/>
+      <c r="B187" s="74"/>
+      <c r="C187" s="74"/>
+      <c r="D187" s="74"/>
+      <c r="E187" s="74"/>
+      <c r="F187" s="74"/>
+      <c r="G187" s="74"/>
       <c r="H187" s="63" t="s">
         <v>131</v>
       </c>
@@ -4756,12 +4759,12 @@
     </row>
     <row r="188" spans="1:11" ht="15" customHeight="1">
       <c r="A188" s="7"/>
-      <c r="B188" s="72"/>
-      <c r="C188" s="72"/>
-      <c r="D188" s="72"/>
-      <c r="E188" s="72"/>
-      <c r="F188" s="72"/>
-      <c r="G188" s="72"/>
+      <c r="B188" s="74"/>
+      <c r="C188" s="74"/>
+      <c r="D188" s="74"/>
+      <c r="E188" s="74"/>
+      <c r="F188" s="74"/>
+      <c r="G188" s="74"/>
       <c r="H188" s="64" t="s">
         <v>89</v>
       </c>
@@ -5514,19 +5517,19 @@
     </row>
     <row r="222" spans="2:15" ht="15" customHeight="1" thickBot="1">
       <c r="E222" s="12"/>
-      <c r="K222" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="L222" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="M222" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="N222" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="O222" s="88" t="s">
+      <c r="K222" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="L222" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="M222" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="N222" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="O222" s="72" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5541,19 +5544,19 @@
       <c r="E223" s="29"/>
       <c r="I223" s="7"/>
       <c r="J223" s="7"/>
-      <c r="K223" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="L223" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="M223" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="N223" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="O223" s="88" t="s">
+      <c r="K223" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="L223" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="M223" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="N223" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="O223" s="72" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5564,19 +5567,19 @@
       <c r="C224" s="7"/>
       <c r="D224" s="7"/>
       <c r="E224" s="29"/>
-      <c r="K224" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="L224" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="M224" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="N224" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="O224" s="88" t="s">
+      <c r="K224" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="L224" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="M224" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="N224" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="O224" s="72" t="s">
         <v>34</v>
       </c>
     </row>
@@ -5586,56 +5589,56 @@
       <c r="C225" s="7"/>
       <c r="D225" s="7"/>
       <c r="E225" s="30"/>
-      <c r="K225" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="L225" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="M225" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="N225" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="O225" s="88" t="s">
+      <c r="K225" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="L225" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="M225" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="N225" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="O225" s="72" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="226" spans="1:15" ht="15" customHeight="1">
       <c r="A226" s="7"/>
-      <c r="B226" s="73" t="s">
+      <c r="B226" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="C226" s="73"/>
-      <c r="D226" s="73"/>
-      <c r="E226" s="73"/>
-      <c r="F226" s="73"/>
-      <c r="G226" s="73"/>
-      <c r="K226" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="L226" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="M226" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="N226" s="88" t="s">
-        <v>34</v>
-      </c>
-      <c r="O226" s="88" t="s">
+      <c r="C226" s="75"/>
+      <c r="D226" s="75"/>
+      <c r="E226" s="75"/>
+      <c r="F226" s="75"/>
+      <c r="G226" s="75"/>
+      <c r="K226" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="L226" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="M226" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="N226" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="O226" s="72" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="227" spans="1:15" ht="15" customHeight="1">
       <c r="A227" s="7"/>
-      <c r="B227" s="73"/>
-      <c r="C227" s="73"/>
-      <c r="D227" s="73"/>
-      <c r="E227" s="73"/>
-      <c r="F227" s="73"/>
-      <c r="G227" s="73"/>
+      <c r="B227" s="75"/>
+      <c r="C227" s="75"/>
+      <c r="D227" s="75"/>
+      <c r="E227" s="75"/>
+      <c r="F227" s="75"/>
+      <c r="G227" s="75"/>
       <c r="K227"/>
       <c r="L227"/>
       <c r="M227"/>
@@ -5644,21 +5647,21 @@
     </row>
     <row r="228" spans="1:15" ht="15" customHeight="1">
       <c r="A228" s="7"/>
-      <c r="B228" s="73"/>
-      <c r="C228" s="73"/>
-      <c r="D228" s="73"/>
-      <c r="E228" s="73"/>
-      <c r="F228" s="73"/>
-      <c r="G228" s="73"/>
+      <c r="B228" s="75"/>
+      <c r="C228" s="75"/>
+      <c r="D228" s="75"/>
+      <c r="E228" s="75"/>
+      <c r="F228" s="75"/>
+      <c r="G228" s="75"/>
     </row>
     <row r="229" spans="1:15" ht="15" customHeight="1">
       <c r="A229" s="7"/>
-      <c r="B229" s="73"/>
-      <c r="C229" s="73"/>
-      <c r="D229" s="73"/>
-      <c r="E229" s="73"/>
-      <c r="F229" s="73"/>
-      <c r="G229" s="73"/>
+      <c r="B229" s="75"/>
+      <c r="C229" s="75"/>
+      <c r="D229" s="75"/>
+      <c r="E229" s="75"/>
+      <c r="F229" s="75"/>
+      <c r="G229" s="75"/>
     </row>
     <row r="230" spans="1:15" ht="15" customHeight="1">
       <c r="B230" s="19"/>
@@ -6459,7 +6462,9 @@
       <c r="D282" s="23">
         <v>12</v>
       </c>
-      <c r="E282" s="5"/>
+      <c r="E282" s="5">
+        <v>26</v>
+      </c>
       <c r="G282" s="39" t="s">
         <v>176</v>
       </c>
@@ -6480,7 +6485,9 @@
       <c r="D283" s="23">
         <v>12</v>
       </c>
-      <c r="E283" s="5"/>
+      <c r="E283" s="5">
+        <v>15</v>
+      </c>
       <c r="G283" s="39" t="s">
         <v>177</v>
       </c>
@@ -6501,7 +6508,9 @@
       <c r="D284" s="23">
         <v>12</v>
       </c>
-      <c r="E284" s="5"/>
+      <c r="E284" s="5">
+        <v>17</v>
+      </c>
       <c r="G284" s="39" t="s">
         <v>178</v>
       </c>
@@ -6522,7 +6531,9 @@
       <c r="D285" s="23">
         <v>12</v>
       </c>
-      <c r="E285" s="5"/>
+      <c r="E285" s="5">
+        <v>12</v>
+      </c>
       <c r="G285" s="39" t="s">
         <v>179</v>
       </c>
@@ -6543,7 +6554,9 @@
       <c r="D286" s="23">
         <v>12</v>
       </c>
-      <c r="E286" s="5"/>
+      <c r="E286" s="5">
+        <v>10</v>
+      </c>
       <c r="G286" s="39" t="s">
         <v>180</v>
       </c>
@@ -6564,7 +6577,9 @@
       <c r="D287" s="23">
         <v>12</v>
       </c>
-      <c r="E287" s="5"/>
+      <c r="E287" s="5">
+        <v>18</v>
+      </c>
       <c r="G287" s="39" t="s">
         <v>181</v>
       </c>
@@ -6585,7 +6600,9 @@
       <c r="D288" s="23">
         <v>12</v>
       </c>
-      <c r="E288" s="5"/>
+      <c r="E288" s="5">
+        <v>33</v>
+      </c>
       <c r="G288" s="39" t="s">
         <v>182</v>
       </c>
@@ -6606,7 +6623,9 @@
       <c r="D289" s="23">
         <v>12</v>
       </c>
-      <c r="E289" s="5"/>
+      <c r="E289" s="5">
+        <v>9</v>
+      </c>
       <c r="G289" s="39" t="s">
         <v>183</v>
       </c>
@@ -6627,7 +6646,9 @@
       <c r="D290" s="23">
         <v>12</v>
       </c>
-      <c r="E290" s="5"/>
+      <c r="E290" s="5">
+        <v>24</v>
+      </c>
       <c r="G290" s="39" t="s">
         <v>184</v>
       </c>
@@ -6648,7 +6669,9 @@
       <c r="D291" s="23">
         <v>12</v>
       </c>
-      <c r="E291" s="5"/>
+      <c r="E291" s="5">
+        <v>5</v>
+      </c>
       <c r="G291" s="39" t="s">
         <v>185</v>
       </c>
@@ -6669,7 +6692,9 @@
       <c r="D292" s="23">
         <v>12</v>
       </c>
-      <c r="E292" s="5"/>
+      <c r="E292" s="5">
+        <v>26</v>
+      </c>
       <c r="G292" s="39" t="s">
         <v>186</v>
       </c>
@@ -6690,7 +6715,9 @@
       <c r="D293" s="23">
         <v>12</v>
       </c>
-      <c r="E293" s="5"/>
+      <c r="E293" s="5">
+        <v>31</v>
+      </c>
       <c r="G293" s="39" t="s">
         <v>187</v>
       </c>
@@ -6711,7 +6738,9 @@
       <c r="D294" s="23">
         <v>12</v>
       </c>
-      <c r="E294" s="5"/>
+      <c r="E294" s="5">
+        <v>31</v>
+      </c>
       <c r="G294" s="39" t="s">
         <v>188</v>
       </c>
@@ -6732,7 +6761,9 @@
       <c r="D295" s="23">
         <v>12</v>
       </c>
-      <c r="E295" s="5"/>
+      <c r="E295" s="5">
+        <v>22</v>
+      </c>
       <c r="G295" s="39" t="s">
         <v>189</v>
       </c>
@@ -6753,7 +6784,9 @@
       <c r="D296" s="23">
         <v>12</v>
       </c>
-      <c r="E296" s="5"/>
+      <c r="E296" s="5">
+        <v>9</v>
+      </c>
       <c r="G296" s="39" t="s">
         <v>190</v>
       </c>
@@ -6774,7 +6807,9 @@
       <c r="D297" s="23">
         <v>12</v>
       </c>
-      <c r="E297" s="5"/>
+      <c r="E297" s="5">
+        <v>42</v>
+      </c>
       <c r="G297" s="39" t="s">
         <v>140</v>
       </c>
@@ -6795,7 +6830,9 @@
       <c r="D298" s="23">
         <v>12</v>
       </c>
-      <c r="E298" s="5"/>
+      <c r="E298" s="5">
+        <v>20</v>
+      </c>
       <c r="G298" s="39" t="s">
         <v>191</v>
       </c>
@@ -6816,7 +6853,9 @@
       <c r="D299" s="23">
         <v>12</v>
       </c>
-      <c r="E299" s="5"/>
+      <c r="E299" s="5">
+        <v>38</v>
+      </c>
       <c r="G299" s="39" t="s">
         <v>192</v>
       </c>
@@ -6837,7 +6876,9 @@
       <c r="D300" s="23">
         <v>12</v>
       </c>
-      <c r="E300" s="5"/>
+      <c r="E300" s="5">
+        <v>15</v>
+      </c>
       <c r="G300" s="39" t="s">
         <v>183</v>
       </c>
@@ -6858,7 +6899,9 @@
       <c r="D301" s="23">
         <v>12</v>
       </c>
-      <c r="E301" s="5"/>
+      <c r="E301" s="5">
+        <v>10</v>
+      </c>
       <c r="G301" s="39" t="s">
         <v>186</v>
       </c>
@@ -6888,7 +6931,7 @@
       </c>
       <c r="E303" s="37" t="str">
         <f>_xlfn.TEXTJOIN(";",FALSE,E282:E301)</f>
-        <v>;;;;;;;;;;;;;;;;;;;</v>
+        <v>26;15;17;12;10;18;33;9;24;5;26;31;31;22;9;42;20;38;15;10</v>
       </c>
     </row>
   </sheetData>
@@ -6913,7 +6956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D843644-E029-4FC8-B4EE-289FDAD015C4}">
   <dimension ref="A1:BW30"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="AQ30" sqref="B2:AQ30"/>
     </sheetView>
   </sheetViews>
@@ -7791,10 +7834,10 @@
       <c r="AO13" s="49"/>
       <c r="AP13" s="49"/>
       <c r="AQ13" s="50"/>
-      <c r="AZ13" s="87" t="s">
+      <c r="AZ13" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="BA13" s="87"/>
+      <c r="BA13" s="89"/>
     </row>
     <row r="14" spans="1:75">
       <c r="A14">
@@ -8926,21 +8969,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A17FE79-6211-4A23-88D4-0F130CF206A1}">
-  <dimension ref="A1:BW30"/>
+  <dimension ref="A1:BJ34"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23:M27"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BA8" sqref="BA8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.44140625" defaultRowHeight="14.4"/>
   <cols>
+    <col min="6" max="25" width="6" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="3.5546875" customWidth="1"/>
-    <col min="29" max="29" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="30" max="36" width="6" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="10.44140625" customWidth="1"/>
     <col min="53" max="53" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="3.77734375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" ht="15" thickBot="1">
+    <row r="1" spans="1:62" ht="15" thickBot="1">
       <c r="B1" t="s">
         <v>31</v>
       </c>
@@ -9107,7 +9156,7 @@
         <v>AQ</v>
       </c>
     </row>
-    <row r="2" spans="1:75">
+    <row r="2" spans="1:62">
       <c r="A2">
         <v>2</v>
       </c>
@@ -9155,8 +9204,19 @@
       <c r="AO2" s="46"/>
       <c r="AP2" s="46"/>
       <c r="AQ2" s="47"/>
-    </row>
-    <row r="3" spans="1:75">
+      <c r="AZ2">
+        <v>117</v>
+      </c>
+      <c r="BA2" t="str">
+        <f>_xlfn.XLOOKUP($AZ$2,Case!$B$280:$B$301,Case!G280:G301)</f>
+        <v>G6</v>
+      </c>
+      <c r="BB2" t="str">
+        <f>_xlfn.XLOOKUP($AZ$2,Case!$B$280:$B$301,Case!H280:H301)</f>
+        <v>🏡</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62">
       <c r="A3">
         <v>3</v>
       </c>
@@ -9215,7 +9275,7 @@
       <c r="AP3" s="49"/>
       <c r="AQ3" s="50"/>
     </row>
-    <row r="4" spans="1:75">
+    <row r="4" spans="1:62">
       <c r="A4">
         <v>4</v>
       </c>
@@ -9264,7 +9324,7 @@
       <c r="AP4" s="49"/>
       <c r="AQ4" s="50"/>
     </row>
-    <row r="5" spans="1:75">
+    <row r="5" spans="1:62">
       <c r="A5">
         <v>5</v>
       </c>
@@ -9331,7 +9391,7 @@
       <c r="AP5" s="49"/>
       <c r="AQ5" s="50"/>
     </row>
-    <row r="6" spans="1:75">
+    <row r="6" spans="1:62">
       <c r="A6">
         <v>6</v>
       </c>
@@ -9341,8 +9401,14 @@
       <c r="E6" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
+      <c r="F6" s="56">
+        <f>IF(F$1&amp;$A6=$BA$2,0,1+MIN(G6,F7,E6,F5))</f>
+        <v>1</v>
+      </c>
+      <c r="G6" s="56">
+        <f>IF(G$1&amp;$A6=$BA$2,0,1+MIN(H6,G7,F6,G5))</f>
+        <v>0</v>
+      </c>
       <c r="H6" s="54"/>
       <c r="I6" s="55"/>
       <c r="J6" s="55"/>
@@ -9363,7 +9429,10 @@
       <c r="W6" s="55"/>
       <c r="X6" s="55"/>
       <c r="Y6" s="55"/>
-      <c r="Z6" s="56"/>
+      <c r="Z6" s="56">
+        <f t="shared" ref="Z6:Z16" ca="1" si="1">IF(Z$1&amp;$A6=$BA$2,0,1+MIN(AA6,Z7,Y6,Z5))</f>
+        <v>41</v>
+      </c>
       <c r="AA6" s="55"/>
       <c r="AB6" s="55"/>
       <c r="AC6" s="55"/>
@@ -9376,15 +9445,26 @@
       </c>
       <c r="AI6" s="55"/>
       <c r="AJ6" s="55"/>
-      <c r="AK6" s="56"/>
+      <c r="AK6" s="56">
+        <f t="shared" ref="AK6:AK8" ca="1" si="2">IF(AK$1&amp;$A6=$BA$2,0,1+MIN(AL6,AK7,AJ6,AK5))</f>
+        <v>52</v>
+      </c>
       <c r="AL6" s="55"/>
       <c r="AM6" s="55"/>
       <c r="AN6" s="54"/>
       <c r="AO6" s="49"/>
       <c r="AP6" s="49"/>
       <c r="AQ6" s="50"/>
-    </row>
-    <row r="7" spans="1:75">
+      <c r="BF6" t="str" cm="1">
+        <f t="array" ref="BF6:BF12">_xlfn.UNIQUE(Case!H280:H301)</f>
+        <v>🏫</v>
+      </c>
+      <c r="BG6">
+        <f ca="1">Z6+1</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62">
       <c r="A7">
         <v>7</v>
       </c>
@@ -9393,12 +9473,30 @@
       <c r="D7" s="54"/>
       <c r="E7" s="55"/>
       <c r="F7" s="55"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
+      <c r="G7" s="56">
+        <f ca="1">IF(G$1&amp;$A7=$BA$2,0,1+MIN(H7,G8,F7,G6))</f>
+        <v>1</v>
+      </c>
+      <c r="H7" s="56">
+        <f t="shared" ref="H7:L17" ca="1" si="3">IF(H$1&amp;$A7=$BA$2,0,1+MIN(I7,H8,G7,H6))</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="J7" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K7" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="L7" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>6</v>
+      </c>
       <c r="M7" s="54"/>
       <c r="N7" s="49"/>
       <c r="O7" s="49"/>
@@ -9416,7 +9514,10 @@
       <c r="W7" s="55"/>
       <c r="X7" s="55"/>
       <c r="Y7" s="55"/>
-      <c r="Z7" s="56"/>
+      <c r="Z7" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>40</v>
+      </c>
       <c r="AA7" s="55"/>
       <c r="AB7" s="55" t="s">
         <v>34</v>
@@ -9433,7 +9534,10 @@
       <c r="AH7" s="55"/>
       <c r="AI7" s="55"/>
       <c r="AJ7" s="55"/>
-      <c r="AK7" s="56"/>
+      <c r="AK7" s="56">
+        <f t="shared" ca="1" si="2"/>
+        <v>51</v>
+      </c>
       <c r="AL7" s="55" t="s">
         <v>34</v>
       </c>
@@ -9442,12 +9546,11 @@
       <c r="AO7" s="49"/>
       <c r="AP7" s="49"/>
       <c r="AQ7" s="50"/>
-      <c r="BW7" t="e" cm="1" vm="1">
-        <f t="array" ref="BW7">_xlfn._xlws.FILTER(BO7:BO175,BP7:BP175&lt;&gt;0)</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="8" spans="1:75">
+      <c r="BF7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62">
       <c r="A8">
         <v>8</v>
       </c>
@@ -9465,7 +9568,10 @@
       </c>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
-      <c r="L8" s="56"/>
+      <c r="L8" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>7</v>
+      </c>
       <c r="M8" s="55" t="s">
         <v>35</v>
       </c>
@@ -9483,26 +9589,69 @@
       </c>
       <c r="X8" s="55"/>
       <c r="Y8" s="55"/>
-      <c r="Z8" s="56"/>
-      <c r="AA8" s="56"/>
-      <c r="AB8" s="56"/>
-      <c r="AC8" s="56"/>
-      <c r="AD8" s="56"/>
-      <c r="AE8" s="56"/>
-      <c r="AF8" s="56"/>
-      <c r="AG8" s="56"/>
-      <c r="AH8" s="56"/>
-      <c r="AI8" s="56"/>
-      <c r="AJ8" s="56"/>
-      <c r="AK8" s="56"/>
+      <c r="Z8" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="AA8" s="56">
+        <f t="shared" ref="AA8" ca="1" si="4">IF(AA$1&amp;$A8=$BA$2,0,1+MIN(AB8,AA9,Z8,AA7))</f>
+        <v>40</v>
+      </c>
+      <c r="AB8" s="56">
+        <f t="shared" ref="AB8" ca="1" si="5">IF(AB$1&amp;$A8=$BA$2,0,1+MIN(AC8,AB9,AA8,AB7))</f>
+        <v>41</v>
+      </c>
+      <c r="AC8" s="56">
+        <f t="shared" ref="AC8" ca="1" si="6">IF(AC$1&amp;$A8=$BA$2,0,1+MIN(AD8,AC9,AB8,AC7))</f>
+        <v>42</v>
+      </c>
+      <c r="AD8" s="56">
+        <f t="shared" ref="AD8" ca="1" si="7">IF(AD$1&amp;$A8=$BA$2,0,1+MIN(AE8,AD9,AC8,AD7))</f>
+        <v>43</v>
+      </c>
+      <c r="AE8" s="56">
+        <f t="shared" ref="AE8" ca="1" si="8">IF(AE$1&amp;$A8=$BA$2,0,1+MIN(AF8,AE9,AD8,AE7))</f>
+        <v>44</v>
+      </c>
+      <c r="AF8" s="56">
+        <f t="shared" ref="AF8" ca="1" si="9">IF(AF$1&amp;$A8=$BA$2,0,1+MIN(AG8,AF9,AE8,AF7))</f>
+        <v>45</v>
+      </c>
+      <c r="AG8" s="56">
+        <f t="shared" ref="AG8" ca="1" si="10">IF(AG$1&amp;$A8=$BA$2,0,1+MIN(AH8,AG9,AF8,AG7))</f>
+        <v>46</v>
+      </c>
+      <c r="AH8" s="56">
+        <f t="shared" ref="AH8" ca="1" si="11">IF(AH$1&amp;$A8=$BA$2,0,1+MIN(AI8,AH9,AG8,AH7))</f>
+        <v>47</v>
+      </c>
+      <c r="AI8" s="56">
+        <f t="shared" ref="AI8" ca="1" si="12">IF(AI$1&amp;$A8=$BA$2,0,1+MIN(AJ8,AI9,AH8,AI7))</f>
+        <v>48</v>
+      </c>
+      <c r="AJ8" s="56">
+        <f t="shared" ref="AJ8" ca="1" si="13">IF(AJ$1&amp;$A8=$BA$2,0,1+MIN(AK8,AJ9,AI8,AJ7))</f>
+        <v>49</v>
+      </c>
+      <c r="AK8" s="56">
+        <f t="shared" ca="1" si="2"/>
+        <v>50</v>
+      </c>
       <c r="AL8" s="55"/>
       <c r="AM8" s="55"/>
       <c r="AN8" s="54"/>
       <c r="AO8" s="49"/>
       <c r="AP8" s="49"/>
       <c r="AQ8" s="50"/>
-    </row>
-    <row r="9" spans="1:75">
+      <c r="BF8" t="str">
+        <v>🏥</v>
+      </c>
+      <c r="BG8">
+        <f ca="1">R21+1</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62">
       <c r="A9">
         <v>9</v>
       </c>
@@ -9522,7 +9671,10 @@
       <c r="I9" s="55"/>
       <c r="J9" s="55"/>
       <c r="K9" s="55"/>
-      <c r="L9" s="56"/>
+      <c r="L9" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>8</v>
+      </c>
       <c r="M9" s="55"/>
       <c r="N9" s="55"/>
       <c r="O9" s="55"/>
@@ -9540,7 +9692,10 @@
       <c r="W9" s="55"/>
       <c r="X9" s="55"/>
       <c r="Y9" s="55"/>
-      <c r="Z9" s="56"/>
+      <c r="Z9" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>38</v>
+      </c>
       <c r="AA9" s="55"/>
       <c r="AB9" s="55"/>
       <c r="AC9" s="55"/>
@@ -9568,8 +9723,15 @@
       <c r="AO9" s="49"/>
       <c r="AP9" s="49"/>
       <c r="AQ9" s="50"/>
-    </row>
-    <row r="10" spans="1:75">
+      <c r="BF9" t="str">
+        <v>🏭</v>
+      </c>
+      <c r="BG9">
+        <f ca="1">P25+1</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:62">
       <c r="A10">
         <v>10</v>
       </c>
@@ -9587,7 +9749,10 @@
       </c>
       <c r="J10" s="55"/>
       <c r="K10" s="55"/>
-      <c r="L10" s="56"/>
+      <c r="L10" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>9</v>
+      </c>
       <c r="M10" s="55" t="s">
         <v>48</v>
       </c>
@@ -9603,7 +9768,10 @@
       <c r="W10" s="55"/>
       <c r="X10" s="55"/>
       <c r="Y10" s="55"/>
-      <c r="Z10" s="56"/>
+      <c r="Z10" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>37</v>
+      </c>
       <c r="AA10" s="55"/>
       <c r="AB10" s="55"/>
       <c r="AC10" s="55"/>
@@ -9627,8 +9795,15 @@
       <c r="AO10" s="49"/>
       <c r="AP10" s="49"/>
       <c r="AQ10" s="50"/>
-    </row>
-    <row r="11" spans="1:75">
+      <c r="BF10" t="str">
+        <v>🏡</v>
+      </c>
+      <c r="BG10">
+        <f ca="1">AB17+1</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62">
       <c r="A11">
         <v>11</v>
       </c>
@@ -9648,7 +9823,10 @@
       <c r="K11" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="56"/>
+      <c r="L11" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>10</v>
+      </c>
       <c r="M11" s="55"/>
       <c r="N11" s="55"/>
       <c r="O11" s="55" t="s">
@@ -9668,7 +9846,10 @@
       </c>
       <c r="X11" s="55"/>
       <c r="Y11" s="55"/>
-      <c r="Z11" s="56"/>
+      <c r="Z11" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>36</v>
+      </c>
       <c r="AA11" s="55"/>
       <c r="AB11" s="55"/>
       <c r="AC11" s="55" t="s">
@@ -9690,8 +9871,15 @@
       <c r="AO11" s="49"/>
       <c r="AP11" s="49"/>
       <c r="AQ11" s="50"/>
-    </row>
-    <row r="12" spans="1:75">
+      <c r="BF11" t="str">
+        <v>🏠</v>
+      </c>
+      <c r="BG11">
+        <f>F6+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62">
       <c r="A12">
         <v>12</v>
       </c>
@@ -9705,7 +9893,10 @@
       <c r="I12" s="55"/>
       <c r="J12" s="55"/>
       <c r="K12" s="55"/>
-      <c r="L12" s="56"/>
+      <c r="L12" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>11</v>
+      </c>
       <c r="M12" s="55"/>
       <c r="N12" s="55"/>
       <c r="O12" s="55"/>
@@ -9721,7 +9912,10 @@
       <c r="W12" s="55"/>
       <c r="X12" s="55"/>
       <c r="Y12" s="55"/>
-      <c r="Z12" s="56"/>
+      <c r="Z12" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>35</v>
+      </c>
       <c r="AA12" s="55"/>
       <c r="AB12" s="55"/>
       <c r="AC12" s="55"/>
@@ -9741,8 +9935,15 @@
         <v>34</v>
       </c>
       <c r="AQ12" s="50"/>
-    </row>
-    <row r="13" spans="1:75" ht="15" thickBot="1">
+      <c r="BF12" t="str">
+        <v>🏦</v>
+      </c>
+      <c r="BG12">
+        <f ca="1">AB17+1</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" ht="15" thickBot="1">
       <c r="A13">
         <v>13</v>
       </c>
@@ -9760,7 +9961,10 @@
       <c r="I13" s="55"/>
       <c r="J13" s="55"/>
       <c r="K13" s="55"/>
-      <c r="L13" s="56"/>
+      <c r="L13" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>12</v>
+      </c>
       <c r="M13" s="55" t="s">
         <v>48</v>
       </c>
@@ -9782,7 +9986,10 @@
       </c>
       <c r="X13" s="55"/>
       <c r="Y13" s="55"/>
-      <c r="Z13" s="56"/>
+      <c r="Z13" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>34</v>
+      </c>
       <c r="AA13" s="55"/>
       <c r="AB13" s="55"/>
       <c r="AC13" s="55"/>
@@ -9806,12 +10013,16 @@
       <c r="AO13" s="49"/>
       <c r="AP13" s="49"/>
       <c r="AQ13" s="50"/>
-      <c r="AZ13" s="87" t="s">
+      <c r="AZ13" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="BA13" s="87"/>
-    </row>
-    <row r="14" spans="1:75">
+      <c r="BA13" s="89"/>
+      <c r="BJ13" cm="1">
+        <f t="array" aca="1" ref="BJ13" ca="1">_xlfn.XLOOKUP(BB2,_xlfn.ANCHORARRAY(BF6),BG6:BG12)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62">
       <c r="A14">
         <v>14</v>
       </c>
@@ -9827,7 +10038,10 @@
       <c r="K14" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="56"/>
+      <c r="L14" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>13</v>
+      </c>
       <c r="M14" s="55"/>
       <c r="N14" s="55"/>
       <c r="O14" s="55"/>
@@ -9849,7 +10063,10 @@
       </c>
       <c r="X14" s="55"/>
       <c r="Y14" s="55"/>
-      <c r="Z14" s="56"/>
+      <c r="Z14" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>33</v>
+      </c>
       <c r="AA14" s="55"/>
       <c r="AB14" s="55"/>
       <c r="AC14" s="55"/>
@@ -9875,8 +10092,12 @@
       <c r="BA14" s="40" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:75">
+      <c r="BE14">
+        <f ca="1">BJ13</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" ht="15.6">
       <c r="A15">
         <v>15</v>
       </c>
@@ -9894,7 +10115,10 @@
       </c>
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
-      <c r="L15" s="56"/>
+      <c r="L15" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>14</v>
+      </c>
       <c r="M15" s="55" t="s">
         <v>48</v>
       </c>
@@ -9918,7 +10142,10 @@
       </c>
       <c r="X15" s="55"/>
       <c r="Y15" s="55"/>
-      <c r="Z15" s="56"/>
+      <c r="Z15" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>32</v>
+      </c>
       <c r="AA15" s="55" t="s">
         <v>34</v>
       </c>
@@ -9946,8 +10173,19 @@
       <c r="BA15" s="42" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:75">
+      <c r="BD15" s="90">
+        <v>111</v>
+      </c>
+      <c r="BE15">
+        <f t="dataTable" ref="BE15:BE34" dt2D="0" dtr="0" r1="AZ2" ca="1"/>
+        <v>26</v>
+      </c>
+      <c r="BG15" cm="1">
+        <f t="array" ref="BG15:BG34">{26;15;17;12;10;18;33;9;24;5;26;31;31;22;9;42;20;38;15;10}</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" ht="15.6">
       <c r="A16">
         <v>16</v>
       </c>
@@ -9963,7 +10201,10 @@
       <c r="K16" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="L16" s="56"/>
+      <c r="L16" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>15</v>
+      </c>
       <c r="M16" s="55"/>
       <c r="N16" s="55"/>
       <c r="O16" s="55" t="s">
@@ -9979,7 +10220,10 @@
       <c r="W16" s="55"/>
       <c r="X16" s="55"/>
       <c r="Y16" s="55"/>
-      <c r="Z16" s="56"/>
+      <c r="Z16" s="56">
+        <f t="shared" ca="1" si="1"/>
+        <v>31</v>
+      </c>
       <c r="AA16" s="55"/>
       <c r="AB16" s="55"/>
       <c r="AC16" s="55"/>
@@ -10003,8 +10247,17 @@
       <c r="BA16" s="42" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:53">
+      <c r="BD16" s="90">
+        <v>112</v>
+      </c>
+      <c r="BE16">
+        <v>15</v>
+      </c>
+      <c r="BG16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:59" ht="15.6">
       <c r="A17">
         <v>17</v>
       </c>
@@ -10020,23 +10273,74 @@
       <c r="I17" s="54"/>
       <c r="J17" s="55"/>
       <c r="K17" s="55"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="56"/>
-      <c r="P17" s="56"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="56"/>
-      <c r="S17" s="56"/>
-      <c r="T17" s="56"/>
-      <c r="U17" s="56"/>
-      <c r="V17" s="56"/>
-      <c r="W17" s="56"/>
-      <c r="X17" s="56"/>
-      <c r="Y17" s="56"/>
-      <c r="Z17" s="56"/>
-      <c r="AA17" s="56"/>
-      <c r="AB17" s="56"/>
+      <c r="L17" s="56">
+        <f t="shared" ca="1" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="M17" s="56">
+        <f t="shared" ref="M17" ca="1" si="14">IF(M$1&amp;$A17=$BA$2,0,1+MIN(N17,M18,L17,M16))</f>
+        <v>17</v>
+      </c>
+      <c r="N17" s="56">
+        <f t="shared" ref="N17" ca="1" si="15">IF(N$1&amp;$A17=$BA$2,0,1+MIN(O17,N18,M17,N16))</f>
+        <v>18</v>
+      </c>
+      <c r="O17" s="56">
+        <f t="shared" ref="O17" ca="1" si="16">IF(O$1&amp;$A17=$BA$2,0,1+MIN(P17,O18,N17,O16))</f>
+        <v>19</v>
+      </c>
+      <c r="P17" s="56">
+        <f t="shared" ref="P17:P25" ca="1" si="17">IF(P$1&amp;$A17=$BA$2,0,1+MIN(Q17,P18,O17,P16))</f>
+        <v>20</v>
+      </c>
+      <c r="Q17" s="56">
+        <f t="shared" ref="Q17" ca="1" si="18">IF(Q$1&amp;$A17=$BA$2,0,1+MIN(R17,Q18,P17,Q16))</f>
+        <v>21</v>
+      </c>
+      <c r="R17" s="56">
+        <f t="shared" ref="R17" ca="1" si="19">IF(R$1&amp;$A17=$BA$2,0,1+MIN(S17,R18,Q17,R16))</f>
+        <v>22</v>
+      </c>
+      <c r="S17" s="56">
+        <f t="shared" ref="S17" ca="1" si="20">IF(S$1&amp;$A17=$BA$2,0,1+MIN(T17,S18,R17,S16))</f>
+        <v>23</v>
+      </c>
+      <c r="T17" s="56">
+        <f t="shared" ref="T17" ca="1" si="21">IF(T$1&amp;$A17=$BA$2,0,1+MIN(U17,T18,S17,T16))</f>
+        <v>24</v>
+      </c>
+      <c r="U17" s="56">
+        <f t="shared" ref="U17" ca="1" si="22">IF(U$1&amp;$A17=$BA$2,0,1+MIN(V17,U18,T17,U16))</f>
+        <v>25</v>
+      </c>
+      <c r="V17" s="56">
+        <f t="shared" ref="V17" ca="1" si="23">IF(V$1&amp;$A17=$BA$2,0,1+MIN(W17,V18,U17,V16))</f>
+        <v>26</v>
+      </c>
+      <c r="W17" s="56">
+        <f t="shared" ref="W17" ca="1" si="24">IF(W$1&amp;$A17=$BA$2,0,1+MIN(X17,W18,V17,W16))</f>
+        <v>27</v>
+      </c>
+      <c r="X17" s="56">
+        <f t="shared" ref="X17" ca="1" si="25">IF(X$1&amp;$A17=$BA$2,0,1+MIN(Y17,X18,W17,X16))</f>
+        <v>28</v>
+      </c>
+      <c r="Y17" s="56">
+        <f t="shared" ref="Y17" ca="1" si="26">IF(Y$1&amp;$A17=$BA$2,0,1+MIN(Z17,Y18,X17,Y16))</f>
+        <v>29</v>
+      </c>
+      <c r="Z17" s="56">
+        <f ca="1">IF(Z$1&amp;$A17=$BA$2,0,1+MIN(AA17,Z18,Y17,Z16))</f>
+        <v>30</v>
+      </c>
+      <c r="AA17" s="56">
+        <f t="shared" ref="AA17" ca="1" si="27">IF(AA$1&amp;$A17=$BA$2,0,1+MIN(AB17,AA18,Z17,AA16))</f>
+        <v>31</v>
+      </c>
+      <c r="AB17" s="56">
+        <f t="shared" ref="AB17" ca="1" si="28">IF(AB$1&amp;$A17=$BA$2,0,1+MIN(AC17,AB18,AA17,AB16))</f>
+        <v>32</v>
+      </c>
       <c r="AC17" s="55" t="s">
         <v>37</v>
       </c>
@@ -10060,8 +10364,17 @@
       <c r="BA17" s="42" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="18" spans="1:53">
+      <c r="BD17" s="90">
+        <v>113</v>
+      </c>
+      <c r="BE17">
+        <v>17</v>
+      </c>
+      <c r="BG17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:59" ht="15.6">
       <c r="A18">
         <v>18</v>
       </c>
@@ -10087,7 +10400,10 @@
       <c r="O18" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="P18" s="56"/>
+      <c r="P18" s="56">
+        <f t="shared" ca="1" si="17"/>
+        <v>21</v>
+      </c>
       <c r="Q18" s="55" t="s">
         <v>48</v>
       </c>
@@ -10130,8 +10446,17 @@
       <c r="BA18" s="42" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="19" spans="1:53">
+      <c r="BD18" s="90">
+        <v>114</v>
+      </c>
+      <c r="BE18">
+        <v>12</v>
+      </c>
+      <c r="BG18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:59" ht="15.6">
       <c r="A19">
         <v>19</v>
       </c>
@@ -10151,7 +10476,10 @@
       <c r="M19" s="55"/>
       <c r="N19" s="55"/>
       <c r="O19" s="55"/>
-      <c r="P19" s="56"/>
+      <c r="P19" s="56">
+        <f ca="1">IF(P$1&amp;$A19=$BA$2,0,1+MIN(Q19,P20,O19,P18))</f>
+        <v>22</v>
+      </c>
       <c r="Q19" s="55"/>
       <c r="R19" s="55"/>
       <c r="S19" s="55"/>
@@ -10200,8 +10528,17 @@
       <c r="BA19" s="42" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="20" spans="1:53">
+      <c r="BD19" s="90">
+        <v>115</v>
+      </c>
+      <c r="BE19">
+        <v>10</v>
+      </c>
+      <c r="BG19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:59" ht="15.6">
       <c r="A20">
         <v>20</v>
       </c>
@@ -10225,7 +10562,10 @@
         <v>48</v>
       </c>
       <c r="O20" s="55"/>
-      <c r="P20" s="56"/>
+      <c r="P20" s="56">
+        <f t="shared" ca="1" si="17"/>
+        <v>23</v>
+      </c>
       <c r="Q20" s="55"/>
       <c r="R20" s="55"/>
       <c r="S20" s="55" t="s">
@@ -10270,8 +10610,17 @@
       <c r="BA20" s="42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="21" spans="1:53">
+      <c r="BD20" s="90">
+        <v>116</v>
+      </c>
+      <c r="BE20">
+        <v>18</v>
+      </c>
+      <c r="BG20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:59" ht="15.6">
       <c r="A21">
         <v>21</v>
       </c>
@@ -10299,9 +10648,18 @@
       <c r="O21" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="P21" s="56"/>
-      <c r="Q21" s="56"/>
-      <c r="R21" s="56"/>
+      <c r="P21" s="56">
+        <f t="shared" ca="1" si="17"/>
+        <v>24</v>
+      </c>
+      <c r="Q21" s="56">
+        <f t="shared" ref="Q21" ca="1" si="29">IF(Q$1&amp;$A21=$BA$2,0,1+MIN(R21,Q22,P21,Q20))</f>
+        <v>25</v>
+      </c>
+      <c r="R21" s="56">
+        <f t="shared" ref="R21" ca="1" si="30">IF(R$1&amp;$A21=$BA$2,0,1+MIN(S21,R22,Q21,R20))</f>
+        <v>26</v>
+      </c>
       <c r="S21" s="55" t="s">
         <v>45</v>
       </c>
@@ -10346,8 +10704,17 @@
       <c r="BA21" s="42" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="22" spans="1:53">
+      <c r="BD21" s="90">
+        <v>117</v>
+      </c>
+      <c r="BE21">
+        <v>33</v>
+      </c>
+      <c r="BG21">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:59" ht="15.6">
       <c r="A22">
         <v>22</v>
       </c>
@@ -10369,7 +10736,10 @@
       <c r="M22" s="55"/>
       <c r="N22" s="55"/>
       <c r="O22" s="55"/>
-      <c r="P22" s="56"/>
+      <c r="P22" s="56">
+        <f t="shared" ca="1" si="17"/>
+        <v>25</v>
+      </c>
       <c r="Q22" s="55"/>
       <c r="R22" s="55"/>
       <c r="S22" s="55" t="s">
@@ -10422,8 +10792,17 @@
       <c r="BA22" s="42" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="23" spans="1:53">
+      <c r="BD22" s="90">
+        <v>118</v>
+      </c>
+      <c r="BE22">
+        <v>9</v>
+      </c>
+      <c r="BG22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:59" ht="15.6">
       <c r="A23">
         <v>23</v>
       </c>
@@ -10449,7 +10828,10 @@
         <v>34</v>
       </c>
       <c r="O23" s="55"/>
-      <c r="P23" s="56"/>
+      <c r="P23" s="56">
+        <f t="shared" ca="1" si="17"/>
+        <v>26</v>
+      </c>
       <c r="Q23" s="55"/>
       <c r="R23" s="55"/>
       <c r="S23" s="55"/>
@@ -10500,8 +10882,17 @@
       <c r="BA23" s="42" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="24" spans="1:53">
+      <c r="BD23" s="90">
+        <v>119</v>
+      </c>
+      <c r="BE23">
+        <v>24</v>
+      </c>
+      <c r="BG23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:59" ht="15.6">
       <c r="A24">
         <v>24</v>
       </c>
@@ -10521,7 +10912,10 @@
       <c r="M24" s="55"/>
       <c r="N24" s="55"/>
       <c r="O24" s="55"/>
-      <c r="P24" s="56"/>
+      <c r="P24" s="56">
+        <f t="shared" ca="1" si="17"/>
+        <v>27</v>
+      </c>
       <c r="Q24" s="55"/>
       <c r="R24" s="55" t="s">
         <v>34</v>
@@ -10570,8 +10964,17 @@
       <c r="BA24" s="42" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="25" spans="1:53">
+      <c r="BD24" s="90">
+        <v>120</v>
+      </c>
+      <c r="BE24">
+        <v>5</v>
+      </c>
+      <c r="BG24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:59" ht="15.6">
       <c r="A25">
         <v>25</v>
       </c>
@@ -10591,7 +10994,10 @@
       <c r="M25" s="55"/>
       <c r="N25" s="55"/>
       <c r="O25" s="55"/>
-      <c r="P25" s="56"/>
+      <c r="P25" s="56">
+        <f ca="1">IF(P$1&amp;$A25=$BA$2,0,1+MIN(Q25,P26,O25,P24))</f>
+        <v>28</v>
+      </c>
       <c r="Q25" s="55"/>
       <c r="R25" s="55"/>
       <c r="S25" s="55"/>
@@ -10634,8 +11040,17 @@
       <c r="BA25" s="42" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="26" spans="1:53">
+      <c r="BD25" s="90">
+        <v>121</v>
+      </c>
+      <c r="BE25">
+        <v>26</v>
+      </c>
+      <c r="BG25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:59" ht="15.6">
       <c r="A26">
         <v>26</v>
       </c>
@@ -10702,8 +11117,17 @@
       <c r="BA26" s="42" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="27" spans="1:53">
+      <c r="BD26" s="90">
+        <v>122</v>
+      </c>
+      <c r="BE26">
+        <v>31</v>
+      </c>
+      <c r="BG26">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:59" ht="15.6">
       <c r="A27">
         <v>27</v>
       </c>
@@ -10758,8 +11182,17 @@
       <c r="BA27" s="42" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="1:53">
+      <c r="BD27" s="90">
+        <v>123</v>
+      </c>
+      <c r="BE27">
+        <v>31</v>
+      </c>
+      <c r="BG27">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:59" ht="15.6">
       <c r="A28">
         <v>28</v>
       </c>
@@ -10814,8 +11247,17 @@
       <c r="BA28" s="42" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:53">
+      <c r="BD28" s="90">
+        <v>124</v>
+      </c>
+      <c r="BE28">
+        <v>22</v>
+      </c>
+      <c r="BG28">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:59" ht="15.6">
       <c r="A29">
         <v>29</v>
       </c>
@@ -10876,8 +11318,17 @@
       <c r="BA29" s="42" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="30" spans="1:53" ht="15" thickBot="1">
+      <c r="BD29" s="90">
+        <v>125</v>
+      </c>
+      <c r="BE29">
+        <v>9</v>
+      </c>
+      <c r="BG29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:59" ht="16.2" thickBot="1">
       <c r="A30">
         <v>30</v>
       </c>
@@ -10930,6 +11381,59 @@
       <c r="BA30" s="44" t="s">
         <v>44</v>
       </c>
+      <c r="BD30" s="90">
+        <v>126</v>
+      </c>
+      <c r="BE30">
+        <v>42</v>
+      </c>
+      <c r="BG30">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:59" ht="15.6">
+      <c r="BD31" s="90">
+        <v>127</v>
+      </c>
+      <c r="BE31">
+        <v>20</v>
+      </c>
+      <c r="BG31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:59" ht="15.6">
+      <c r="BD32" s="90">
+        <v>128</v>
+      </c>
+      <c r="BE32">
+        <v>18</v>
+      </c>
+      <c r="BG32">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="56:59" ht="15.6">
+      <c r="BD33" s="90">
+        <v>129</v>
+      </c>
+      <c r="BE33">
+        <v>15</v>
+      </c>
+      <c r="BG33">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="56:59" ht="15.6">
+      <c r="BD34" s="90">
+        <v>130</v>
+      </c>
+      <c r="BE34">
+        <v>10</v>
+      </c>
+      <c r="BG34">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -10990,48 +11494,48 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="72"/>
-      <c r="F6" s="72"/>
-      <c r="G6" s="72"/>
+      <c r="B6" s="74"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="74"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="74"/>
+      <c r="G6" s="74"/>
       <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="72"/>
-      <c r="E7" s="72"/>
-      <c r="F7" s="72"/>
-      <c r="G7" s="72"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="72"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="18" t="s">

</xml_diff>

<commit_message>
Looking at circular calculation
</commit_message>
<xml_diff>
--- a/The_Maps_Case.xlsx
+++ b/The_Maps_Case.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D6B0B6-F4CF-48A0-9B79-6A5C1A4A2B80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE7BB11-1436-4F7A-903C-828D1C58DD22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4D370DF4-3C71-4D6D-AE9D-E6E375992910}"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <definedName name="_m">Map_Copy!$B$2:$AQ$30</definedName>
     <definedName name="_map">The_Map_for_the_Training_Case!$B$2:$AQ$30</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="211">
   <si>
     <t>Case Author</t>
   </si>
@@ -2042,8 +2042,8 @@
   </sheetPr>
   <dimension ref="A1:O303"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A275" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H283" sqref="H283"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A298" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G309" sqref="G309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18" defaultRowHeight="14.4"/>
@@ -8971,8 +8971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A17FE79-6211-4A23-88D4-0F130CF206A1}">
   <dimension ref="A1:BJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BA8" sqref="BA8"/>
+    <sheetView topLeftCell="P1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.44140625" defaultRowHeight="14.4"/>
@@ -9204,16 +9204,16 @@
       <c r="AO2" s="46"/>
       <c r="AP2" s="46"/>
       <c r="AQ2" s="47"/>
-      <c r="AZ2">
-        <v>117</v>
+      <c r="AZ2" t="s">
+        <v>23</v>
       </c>
       <c r="BA2" t="str">
         <f>_xlfn.XLOOKUP($AZ$2,Case!$B$280:$B$301,Case!G280:G301)</f>
-        <v>G6</v>
+        <v>Z8</v>
       </c>
       <c r="BB2" t="str">
         <f>_xlfn.XLOOKUP($AZ$2,Case!$B$280:$B$301,Case!H280:H301)</f>
-        <v>🏡</v>
+        <v>🏫</v>
       </c>
     </row>
     <row r="3" spans="1:62">
@@ -9402,12 +9402,12 @@
         <v>36</v>
       </c>
       <c r="F6" s="56">
-        <f>IF(F$1&amp;$A6=$BA$2,0,1+MIN(G6,F7,E6,F5))</f>
-        <v>1</v>
+        <f ca="1">IF(F$1&amp;$A6=$BA$2,0,1+MIN(G6,F7,E6,F5))</f>
+        <v>40</v>
       </c>
       <c r="G6" s="56">
-        <f>IF(G$1&amp;$A6=$BA$2,0,1+MIN(H6,G7,F6,G5))</f>
-        <v>0</v>
+        <f ca="1">IF(G$1&amp;$A6=$BA$2,0,1+MIN(H6,G7,F6,G5))</f>
+        <v>39</v>
       </c>
       <c r="H6" s="54"/>
       <c r="I6" s="55"/>
@@ -9431,7 +9431,7 @@
       <c r="Y6" s="55"/>
       <c r="Z6" s="56">
         <f t="shared" ref="Z6:Z16" ca="1" si="1">IF(Z$1&amp;$A6=$BA$2,0,1+MIN(AA6,Z7,Y6,Z5))</f>
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="AA6" s="55"/>
       <c r="AB6" s="55"/>
@@ -9447,7 +9447,7 @@
       <c r="AJ6" s="55"/>
       <c r="AK6" s="56">
         <f t="shared" ref="AK6:AK8" ca="1" si="2">IF(AK$1&amp;$A6=$BA$2,0,1+MIN(AL6,AK7,AJ6,AK5))</f>
-        <v>52</v>
+        <v>13</v>
       </c>
       <c r="AL6" s="55"/>
       <c r="AM6" s="55"/>
@@ -9461,7 +9461,7 @@
       </c>
       <c r="BG6">
         <f ca="1">Z6+1</f>
-        <v>42</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:62">
@@ -9475,27 +9475,27 @@
       <c r="F7" s="55"/>
       <c r="G7" s="56">
         <f ca="1">IF(G$1&amp;$A7=$BA$2,0,1+MIN(H7,G8,F7,G6))</f>
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="H7" s="56">
         <f t="shared" ref="H7:L17" ca="1" si="3">IF(H$1&amp;$A7=$BA$2,0,1+MIN(I7,H8,G7,H6))</f>
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="I7" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="J7" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="K7" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="L7" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="M7" s="54"/>
       <c r="N7" s="49"/>
@@ -9516,7 +9516,7 @@
       <c r="Y7" s="55"/>
       <c r="Z7" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="AA7" s="55"/>
       <c r="AB7" s="55" t="s">
@@ -9536,7 +9536,7 @@
       <c r="AJ7" s="55"/>
       <c r="AK7" s="56">
         <f t="shared" ca="1" si="2"/>
-        <v>51</v>
+        <v>12</v>
       </c>
       <c r="AL7" s="55" t="s">
         <v>34</v>
@@ -9570,7 +9570,7 @@
       <c r="K8" s="55"/>
       <c r="L8" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="M8" s="55" t="s">
         <v>35</v>
@@ -9590,52 +9590,52 @@
       <c r="X8" s="55"/>
       <c r="Y8" s="55"/>
       <c r="Z8" s="56">
-        <f t="shared" ca="1" si="1"/>
-        <v>39</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="AA8" s="56">
         <f t="shared" ref="AA8" ca="1" si="4">IF(AA$1&amp;$A8=$BA$2,0,1+MIN(AB8,AA9,Z8,AA7))</f>
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="AB8" s="56">
         <f t="shared" ref="AB8" ca="1" si="5">IF(AB$1&amp;$A8=$BA$2,0,1+MIN(AC8,AB9,AA8,AB7))</f>
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="AC8" s="56">
         <f t="shared" ref="AC8" ca="1" si="6">IF(AC$1&amp;$A8=$BA$2,0,1+MIN(AD8,AC9,AB8,AC7))</f>
-        <v>42</v>
+        <v>3</v>
       </c>
       <c r="AD8" s="56">
         <f t="shared" ref="AD8" ca="1" si="7">IF(AD$1&amp;$A8=$BA$2,0,1+MIN(AE8,AD9,AC8,AD7))</f>
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="AE8" s="56">
         <f t="shared" ref="AE8" ca="1" si="8">IF(AE$1&amp;$A8=$BA$2,0,1+MIN(AF8,AE9,AD8,AE7))</f>
-        <v>44</v>
+        <v>5</v>
       </c>
       <c r="AF8" s="56">
         <f t="shared" ref="AF8" ca="1" si="9">IF(AF$1&amp;$A8=$BA$2,0,1+MIN(AG8,AF9,AE8,AF7))</f>
-        <v>45</v>
+        <v>6</v>
       </c>
       <c r="AG8" s="56">
         <f t="shared" ref="AG8" ca="1" si="10">IF(AG$1&amp;$A8=$BA$2,0,1+MIN(AH8,AG9,AF8,AG7))</f>
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="AH8" s="56">
         <f t="shared" ref="AH8" ca="1" si="11">IF(AH$1&amp;$A8=$BA$2,0,1+MIN(AI8,AH9,AG8,AH7))</f>
-        <v>47</v>
+        <v>8</v>
       </c>
       <c r="AI8" s="56">
         <f t="shared" ref="AI8" ca="1" si="12">IF(AI$1&amp;$A8=$BA$2,0,1+MIN(AJ8,AI9,AH8,AI7))</f>
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="AJ8" s="56">
         <f t="shared" ref="AJ8" ca="1" si="13">IF(AJ$1&amp;$A8=$BA$2,0,1+MIN(AK8,AJ9,AI8,AJ7))</f>
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="AK8" s="56">
         <f t="shared" ca="1" si="2"/>
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="AL8" s="55"/>
       <c r="AM8" s="55"/>
@@ -9648,7 +9648,7 @@
       </c>
       <c r="BG8">
         <f ca="1">R21+1</f>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:62">
@@ -9673,7 +9673,7 @@
       <c r="K9" s="55"/>
       <c r="L9" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="M9" s="55"/>
       <c r="N9" s="55"/>
@@ -9694,7 +9694,7 @@
       <c r="Y9" s="55"/>
       <c r="Z9" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="AA9" s="55"/>
       <c r="AB9" s="55"/>
@@ -9728,7 +9728,7 @@
       </c>
       <c r="BG9">
         <f ca="1">P25+1</f>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:62">
@@ -9751,7 +9751,7 @@
       <c r="K10" s="55"/>
       <c r="L10" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="M10" s="55" t="s">
         <v>48</v>
@@ -9770,7 +9770,7 @@
       <c r="Y10" s="55"/>
       <c r="Z10" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>37</v>
+        <v>2</v>
       </c>
       <c r="AA10" s="55"/>
       <c r="AB10" s="55"/>
@@ -9800,7 +9800,7 @@
       </c>
       <c r="BG10">
         <f ca="1">AB17+1</f>
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:62">
@@ -9825,7 +9825,7 @@
       </c>
       <c r="L11" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="M11" s="55"/>
       <c r="N11" s="55"/>
@@ -9848,7 +9848,7 @@
       <c r="Y11" s="55"/>
       <c r="Z11" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="AA11" s="55"/>
       <c r="AB11" s="55"/>
@@ -9875,8 +9875,8 @@
         <v>🏠</v>
       </c>
       <c r="BG11">
-        <f>F6+1</f>
-        <v>2</v>
+        <f ca="1">F6+1</f>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:62">
@@ -9895,7 +9895,7 @@
       <c r="K12" s="55"/>
       <c r="L12" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="M12" s="55"/>
       <c r="N12" s="55"/>
@@ -9914,7 +9914,7 @@
       <c r="Y12" s="55"/>
       <c r="Z12" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>35</v>
+        <v>4</v>
       </c>
       <c r="AA12" s="55"/>
       <c r="AB12" s="55"/>
@@ -9940,7 +9940,7 @@
       </c>
       <c r="BG12">
         <f ca="1">AB17+1</f>
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:62" ht="15" thickBot="1">
@@ -9963,7 +9963,7 @@
       <c r="K13" s="55"/>
       <c r="L13" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="M13" s="55" t="s">
         <v>48</v>
@@ -9988,7 +9988,7 @@
       <c r="Y13" s="55"/>
       <c r="Z13" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="AA13" s="55"/>
       <c r="AB13" s="55"/>
@@ -10019,7 +10019,7 @@
       <c r="BA13" s="89"/>
       <c r="BJ13" cm="1">
         <f t="array" aca="1" ref="BJ13" ca="1">_xlfn.XLOOKUP(BB2,_xlfn.ANCHORARRAY(BF6),BG6:BG12)</f>
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:62">
@@ -10040,7 +10040,7 @@
       </c>
       <c r="L14" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="M14" s="55"/>
       <c r="N14" s="55"/>
@@ -10065,7 +10065,7 @@
       <c r="Y14" s="55"/>
       <c r="Z14" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="AA14" s="55"/>
       <c r="AB14" s="55"/>
@@ -10094,7 +10094,7 @@
       </c>
       <c r="BE14">
         <f ca="1">BJ13</f>
-        <v>33</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:62" ht="15.6">
@@ -10117,7 +10117,7 @@
       <c r="K15" s="55"/>
       <c r="L15" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="M15" s="55" t="s">
         <v>48</v>
@@ -10144,7 +10144,7 @@
       <c r="Y15" s="55"/>
       <c r="Z15" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="AA15" s="55" t="s">
         <v>34</v>
@@ -10203,7 +10203,7 @@
       </c>
       <c r="L16" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="M16" s="55"/>
       <c r="N16" s="55"/>
@@ -10222,7 +10222,7 @@
       <c r="Y16" s="55"/>
       <c r="Z16" s="56">
         <f t="shared" ca="1" si="1"/>
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="AA16" s="55"/>
       <c r="AB16" s="55"/>
@@ -10275,71 +10275,71 @@
       <c r="K17" s="55"/>
       <c r="L17" s="56">
         <f t="shared" ca="1" si="3"/>
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="M17" s="56">
         <f t="shared" ref="M17" ca="1" si="14">IF(M$1&amp;$A17=$BA$2,0,1+MIN(N17,M18,L17,M16))</f>
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="N17" s="56">
         <f t="shared" ref="N17" ca="1" si="15">IF(N$1&amp;$A17=$BA$2,0,1+MIN(O17,N18,M17,N16))</f>
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="O17" s="56">
         <f t="shared" ref="O17" ca="1" si="16">IF(O$1&amp;$A17=$BA$2,0,1+MIN(P17,O18,N17,O16))</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P17" s="56">
         <f t="shared" ref="P17:P25" ca="1" si="17">IF(P$1&amp;$A17=$BA$2,0,1+MIN(Q17,P18,O17,P16))</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q17" s="56">
         <f t="shared" ref="Q17" ca="1" si="18">IF(Q$1&amp;$A17=$BA$2,0,1+MIN(R17,Q18,P17,Q16))</f>
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="R17" s="56">
         <f t="shared" ref="R17" ca="1" si="19">IF(R$1&amp;$A17=$BA$2,0,1+MIN(S17,R18,Q17,R16))</f>
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="S17" s="56">
         <f t="shared" ref="S17" ca="1" si="20">IF(S$1&amp;$A17=$BA$2,0,1+MIN(T17,S18,R17,S16))</f>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="T17" s="56">
         <f t="shared" ref="T17" ca="1" si="21">IF(T$1&amp;$A17=$BA$2,0,1+MIN(U17,T18,S17,T16))</f>
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="U17" s="56">
         <f t="shared" ref="U17" ca="1" si="22">IF(U$1&amp;$A17=$BA$2,0,1+MIN(V17,U18,T17,U16))</f>
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="V17" s="56">
         <f t="shared" ref="V17" ca="1" si="23">IF(V$1&amp;$A17=$BA$2,0,1+MIN(W17,V18,U17,V16))</f>
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="W17" s="56">
         <f t="shared" ref="W17" ca="1" si="24">IF(W$1&amp;$A17=$BA$2,0,1+MIN(X17,W18,V17,W16))</f>
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="X17" s="56">
         <f t="shared" ref="X17" ca="1" si="25">IF(X$1&amp;$A17=$BA$2,0,1+MIN(Y17,X18,W17,X16))</f>
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="Y17" s="56">
         <f t="shared" ref="Y17" ca="1" si="26">IF(Y$1&amp;$A17=$BA$2,0,1+MIN(Z17,Y18,X17,Y16))</f>
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="Z17" s="56">
         <f ca="1">IF(Z$1&amp;$A17=$BA$2,0,1+MIN(AA17,Z18,Y17,Z16))</f>
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="AA17" s="56">
         <f t="shared" ref="AA17" ca="1" si="27">IF(AA$1&amp;$A17=$BA$2,0,1+MIN(AB17,AA18,Z17,AA16))</f>
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="AB17" s="56">
         <f t="shared" ref="AB17" ca="1" si="28">IF(AB$1&amp;$A17=$BA$2,0,1+MIN(AC17,AB18,AA17,AB16))</f>
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="AC17" s="55" t="s">
         <v>37</v>
@@ -10402,7 +10402,7 @@
       </c>
       <c r="P18" s="56">
         <f t="shared" ca="1" si="17"/>
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="Q18" s="55" t="s">
         <v>48</v>
@@ -10478,7 +10478,7 @@
       <c r="O19" s="55"/>
       <c r="P19" s="56">
         <f ca="1">IF(P$1&amp;$A19=$BA$2,0,1+MIN(Q19,P20,O19,P18))</f>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="Q19" s="55"/>
       <c r="R19" s="55"/>
@@ -10564,7 +10564,7 @@
       <c r="O20" s="55"/>
       <c r="P20" s="56">
         <f t="shared" ca="1" si="17"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q20" s="55"/>
       <c r="R20" s="55"/>
@@ -10650,15 +10650,15 @@
       </c>
       <c r="P21" s="56">
         <f t="shared" ca="1" si="17"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" s="56">
         <f t="shared" ref="Q21" ca="1" si="29">IF(Q$1&amp;$A21=$BA$2,0,1+MIN(R21,Q22,P21,Q20))</f>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R21" s="56">
         <f t="shared" ref="R21" ca="1" si="30">IF(R$1&amp;$A21=$BA$2,0,1+MIN(S21,R22,Q21,R20))</f>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="S21" s="55" t="s">
         <v>45</v>
@@ -10738,7 +10738,7 @@
       <c r="O22" s="55"/>
       <c r="P22" s="56">
         <f t="shared" ca="1" si="17"/>
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q22" s="55"/>
       <c r="R22" s="55"/>
@@ -10830,7 +10830,7 @@
       <c r="O23" s="55"/>
       <c r="P23" s="56">
         <f t="shared" ca="1" si="17"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q23" s="55"/>
       <c r="R23" s="55"/>
@@ -10914,7 +10914,7 @@
       <c r="O24" s="55"/>
       <c r="P24" s="56">
         <f t="shared" ca="1" si="17"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="Q24" s="55"/>
       <c r="R24" s="55" t="s">
@@ -10996,7 +10996,7 @@
       <c r="O25" s="55"/>
       <c r="P25" s="56">
         <f ca="1">IF(P$1&amp;$A25=$BA$2,0,1+MIN(Q25,P26,O25,P24))</f>
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Q25" s="55"/>
       <c r="R25" s="55"/>

</xml_diff>